<commit_message>
changed pinnacle html class names
</commit_message>
<xml_diff>
--- a/betting spreadsheet.xlsx
+++ b/betting spreadsheet.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Desktop\betting-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E450799B-1CD5-4820-9A13-249A35C6158B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84BC3C-7087-402F-8108-9A5D9BC5F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$108</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$130</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="251">
   <si>
     <t>Date</t>
   </si>
@@ -95,18 +95,12 @@
     <t>Bet Name</t>
   </si>
   <si>
-    <t>New York Jets -3</t>
-  </si>
-  <si>
     <t>Toronto Raptors -1.5</t>
   </si>
   <si>
     <t>Boston Celtics vs Miami Heat</t>
   </si>
   <si>
-    <t>Miami Heat -2</t>
-  </si>
-  <si>
     <t>Richard Gasquet vs Felix Auger Aliassime</t>
   </si>
   <si>
@@ -644,9 +638,6 @@
     <t>Carolina Panthers</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Arizona Cardinals vs New England Patriots</t>
   </si>
   <si>
@@ -744,6 +735,63 @@
   </si>
   <si>
     <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
+    <t>Yale vs Fairfield</t>
+  </si>
+  <si>
+    <t>Fairfield +3.0</t>
+  </si>
+  <si>
+    <t>UC San Diego vs San Diego</t>
+  </si>
+  <si>
+    <t>UC San Diego +4.5</t>
+  </si>
+  <si>
+    <t>Liberty vs Oral Roberts</t>
+  </si>
+  <si>
+    <t>Liberty</t>
+  </si>
+  <si>
+    <t>Miami Heat vs Indiana Pacers</t>
+  </si>
+  <si>
+    <t>Miami Heat -6.0</t>
+  </si>
+  <si>
+    <t>Miami Heat -2.0</t>
+  </si>
+  <si>
+    <t>New York Jets -3.0</t>
+  </si>
+  <si>
+    <t>UC San Diego +3.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams vs Green Bay Packers</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams +7.5</t>
+  </si>
+  <si>
+    <t>MD Baltimore County vs Loyola Maryland</t>
+  </si>
+  <si>
+    <t>Loyola Maryland</t>
+  </si>
+  <si>
+    <t>Furman vs NC State</t>
+  </si>
+  <si>
+    <t>Furman +4.0</t>
+  </si>
+  <si>
+    <t>Anaheim Ducks vs Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>Toronto Maple Leafs -2.5</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1075,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$108</c:f>
+              <c:f>Sheet1!$K$2:$K$130</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="107"/>
+                <c:ptCount val="129"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -1314,43 +1362,82 @@
                   <c:v>35.70000000000001</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>35.70000000000001</c:v>
+                  <c:v>36.610000000000007</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>33.70000000000001</c:v>
+                  <c:v>34.610000000000007</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>34.13000000000001</c:v>
+                  <c:v>35.040000000000006</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>36.430000000000007</c:v>
+                  <c:v>37.340000000000003</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>35.430000000000007</c:v>
+                  <c:v>36.340000000000003</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>36.300000000000004</c:v>
+                  <c:v>37.21</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>37.440000000000005</c:v>
+                  <c:v>38.35</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>36.440000000000005</c:v>
+                  <c:v>37.35</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>35.440000000000005</c:v>
+                  <c:v>36.35</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>34.440000000000005</c:v>
+                  <c:v>35.35</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>33.440000000000005</c:v>
+                  <c:v>34.35</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>34.640000000000008</c:v>
+                  <c:v>35.550000000000004</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>32.640000000000008</c:v>
+                  <c:v>33.550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>32.550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>30.550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>31.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>30.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>29.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>28.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>27.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>26.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>25.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>24.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>23.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>22.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>23.850000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1558,7 +1645,7 @@
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="waterfall" uniqueId="{AC6488E2-B87F-49E6-98C0-CC41BB5305B6}">
+        <cx:series layoutId="waterfall" uniqueId="{AEDEC493-1E32-4D36-99EF-67EAF86BF7E1}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:subtotals/>
@@ -3093,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9706E5D-ABEE-4E65-AA0D-26913405A8B0}">
   <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3163,7 +3250,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>241</v>
       </c>
       <c r="E2" s="6">
         <v>150</v>
@@ -3190,7 +3277,7 @@
       </c>
       <c r="M2" s="13">
         <f>SUM(J2:J130)</f>
-        <v>30.890000000000008</v>
+        <v>23.850000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3204,7 +3291,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6">
         <v>145</v>
@@ -3235,13 +3322,13 @@
         <v>44855</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>21</v>
+        <v>240</v>
       </c>
       <c r="E4" s="6">
         <v>145</v>
@@ -3272,13 +3359,13 @@
         <v>44856</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="6">
         <v>-105</v>
@@ -3309,13 +3396,13 @@
         <v>44856</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="E6" s="6">
         <v>115</v>
@@ -3346,13 +3433,13 @@
         <v>44857</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="E7" s="6">
         <v>-130</v>
@@ -3383,13 +3470,13 @@
         <v>44858</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="E8" s="6">
         <v>170</v>
@@ -3420,13 +3507,13 @@
         <v>44858</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="6">
         <v>120</v>
@@ -3457,13 +3544,13 @@
         <v>44858</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="E10" s="6">
         <v>-105</v>
@@ -3494,13 +3581,13 @@
         <v>44859</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="6">
         <v>-105</v>
@@ -3531,13 +3618,13 @@
         <v>44859</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="E12" s="6">
         <v>120</v>
@@ -3568,13 +3655,13 @@
         <v>44859</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="E13" s="6">
         <v>110</v>
@@ -3605,13 +3692,13 @@
         <v>44859</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="E14" s="6">
         <v>140</v>
@@ -3642,13 +3729,13 @@
         <v>44877</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="6">
         <v>110</v>
@@ -3679,13 +3766,13 @@
         <v>44878</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="E16" s="6">
         <v>125</v>
@@ -3716,13 +3803,13 @@
         <v>44878</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="6">
         <v>105</v>
@@ -3753,13 +3840,13 @@
         <v>44878</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E18" s="6">
         <v>-105</v>
@@ -3790,13 +3877,13 @@
         <v>44878</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E19" s="6">
         <v>105</v>
@@ -3827,13 +3914,13 @@
         <v>44879</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="6">
         <v>425</v>
@@ -3864,13 +3951,13 @@
         <v>44879</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E21" s="6">
         <v>170</v>
@@ -3901,13 +3988,13 @@
         <v>44879</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E22" s="6">
         <v>1000</v>
@@ -3938,13 +4025,13 @@
         <v>44879</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23" s="6">
         <v>160</v>
@@ -3975,13 +4062,13 @@
         <v>44879</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="6">
         <v>725</v>
@@ -4013,13 +4100,13 @@
         <v>44881</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E25" s="6">
         <v>425</v>
@@ -4051,13 +4138,13 @@
         <v>44881</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E26" s="6">
         <v>-140</v>
@@ -4089,13 +4176,13 @@
         <v>44881</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E27" s="6">
         <v>110</v>
@@ -4127,13 +4214,13 @@
         <v>44881</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E28" s="6">
         <v>275</v>
@@ -4165,13 +4252,13 @@
         <v>44881</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E29" s="6">
         <v>-200</v>
@@ -4202,13 +4289,13 @@
         <v>44881</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E30" s="6">
         <v>250</v>
@@ -4239,13 +4326,13 @@
         <v>44881</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="6">
         <v>-140</v>
@@ -4276,13 +4363,13 @@
         <v>44882</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" s="6">
         <v>400</v>
@@ -4313,13 +4400,13 @@
         <v>44882</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E33" s="6">
         <v>175</v>
@@ -4350,13 +4437,13 @@
         <v>44883</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E34" s="6">
         <v>120</v>
@@ -4387,13 +4474,13 @@
         <v>44883</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E35" s="6">
         <v>650</v>
@@ -4424,13 +4511,13 @@
         <v>44883</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E36" s="6">
         <v>-105</v>
@@ -4461,13 +4548,13 @@
         <v>44883</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E37" s="6">
         <v>-105</v>
@@ -4501,10 +4588,10 @@
         <v>15</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E38" s="6">
         <v>-105</v>
@@ -4535,13 +4622,13 @@
         <v>44883</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E39" s="6">
         <v>390</v>
@@ -4572,13 +4659,13 @@
         <v>44885</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" s="6">
         <v>450</v>
@@ -4609,13 +4696,13 @@
         <v>44885</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E41" s="6">
         <v>275</v>
@@ -4646,13 +4733,13 @@
         <v>44885</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E42" s="6">
         <v>-150</v>
@@ -4683,13 +4770,13 @@
         <v>44885</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E43" s="6">
         <v>125</v>
@@ -4720,13 +4807,13 @@
         <v>44885</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E44" s="6">
         <v>1300</v>
@@ -4757,13 +4844,13 @@
         <v>44885</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E45" s="6">
         <v>145</v>
@@ -4794,13 +4881,13 @@
         <v>44885</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="E46" s="6">
         <v>140</v>
@@ -4831,13 +4918,13 @@
         <v>44886</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E47" s="6">
         <v>525</v>
@@ -4868,13 +4955,13 @@
         <v>44886</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E48" s="6">
         <v>175</v>
@@ -4905,13 +4992,13 @@
         <v>44886</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E49" s="6">
         <v>105</v>
@@ -4942,13 +5029,13 @@
         <v>44886</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E50" s="6">
         <v>1050</v>
@@ -4979,13 +5066,13 @@
         <v>44886</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E51" s="6">
         <v>375</v>
@@ -5016,13 +5103,13 @@
         <v>44886</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E52" s="6">
         <v>125</v>
@@ -5053,13 +5140,13 @@
         <v>44886</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E53" s="6">
         <v>-110</v>
@@ -5090,13 +5177,13 @@
         <v>44886</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E54" s="6">
         <v>160</v>
@@ -5127,13 +5214,13 @@
         <v>44887</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>126</v>
       </c>
       <c r="E55" s="6">
         <v>-110</v>
@@ -5164,13 +5251,13 @@
         <v>44887</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E56" s="6">
         <v>130</v>
@@ -5201,13 +5288,13 @@
         <v>44887</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E57" s="6">
         <v>-130</v>
@@ -5238,13 +5325,13 @@
         <v>44887</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E58" s="6">
         <v>-180</v>
@@ -5275,13 +5362,13 @@
         <v>44887</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E59" s="6">
         <v>-245</v>
@@ -5312,13 +5399,13 @@
         <v>44887</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E60" s="6">
         <v>-260</v>
@@ -5349,13 +5436,13 @@
         <v>44888</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E61" s="6">
         <v>150</v>
@@ -5386,13 +5473,13 @@
         <v>44888</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E62" s="6">
         <v>-140</v>
@@ -5423,13 +5510,13 @@
         <v>44888</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E63" s="6">
         <v>-110</v>
@@ -5460,13 +5547,13 @@
         <v>44888</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E64" s="6">
         <v>-210</v>
@@ -5497,13 +5584,13 @@
         <v>44890</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E65" s="6">
         <v>150</v>
@@ -5525,7 +5612,7 @@
         <v>-1</v>
       </c>
       <c r="K65" s="11">
-        <f t="shared" ref="K65:K112" si="4">K64+J65</f>
+        <f t="shared" ref="K65:K121" si="4">K64+J65</f>
         <v>46.630000000000017</v>
       </c>
     </row>
@@ -5534,13 +5621,13 @@
         <v>44891</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E66" s="6">
         <v>265</v>
@@ -5571,13 +5658,13 @@
         <v>44891</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E67" s="6">
         <v>160</v>
@@ -5608,13 +5695,13 @@
         <v>44892</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E68" s="6">
         <v>215</v>
@@ -5645,13 +5732,13 @@
         <v>44892</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E69" s="6">
         <v>-135</v>
@@ -5682,13 +5769,13 @@
         <v>44892</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E70" s="6">
         <v>150</v>
@@ -5719,13 +5806,13 @@
         <v>44892</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E71" s="6">
         <v>1400</v>
@@ -5756,13 +5843,13 @@
         <v>44892</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E72" s="6">
         <v>230</v>
@@ -5793,13 +5880,13 @@
         <v>44893</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E73" s="6">
         <v>-125</v>
@@ -5814,7 +5901,7 @@
         <v>1.8</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J73" s="11">
         <v>0</v>
@@ -5829,13 +5916,13 @@
         <v>44893</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E74" s="6">
         <v>-115</v>
@@ -5866,13 +5953,13 @@
         <v>44893</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E75" s="6">
         <v>450</v>
@@ -5903,13 +5990,13 @@
         <v>44893</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E76" s="6">
         <v>390</v>
@@ -5940,13 +6027,13 @@
         <v>44893</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E77" s="6">
         <v>-235</v>
@@ -5977,13 +6064,13 @@
         <v>44893</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E78" s="6">
         <v>-195</v>
@@ -6014,13 +6101,13 @@
         <v>44893</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E79" s="6">
         <v>500</v>
@@ -6051,13 +6138,13 @@
         <v>44893</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E80" s="6">
         <v>140</v>
@@ -6088,13 +6175,13 @@
         <v>44894</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E81" s="6">
         <v>110</v>
@@ -6125,13 +6212,13 @@
         <v>44894</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E82" s="6">
         <v>125</v>
@@ -6162,13 +6249,13 @@
         <v>44894</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E83" s="6">
         <v>250</v>
@@ -6199,13 +6286,13 @@
         <v>44895</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E84" s="6">
         <v>165</v>
@@ -6236,13 +6323,13 @@
         <v>44895</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E85" s="6">
         <v>140</v>
@@ -6273,13 +6360,13 @@
         <v>44895</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E86" s="6">
         <v>165</v>
@@ -6310,13 +6397,13 @@
         <v>44895</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E87" s="6">
         <v>1000</v>
@@ -6347,13 +6434,13 @@
         <v>44897</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E88" s="6">
         <v>375</v>
@@ -6384,13 +6471,13 @@
         <v>44898</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E89" s="6">
         <v>1250</v>
@@ -6421,13 +6508,13 @@
         <v>44898</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E90" s="6">
         <v>265</v>
@@ -6458,13 +6545,13 @@
         <v>44898</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E91" s="6">
         <v>255</v>
@@ -6495,13 +6582,13 @@
         <v>44898</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E92" s="6">
         <v>135</v>
@@ -6532,13 +6619,13 @@
         <v>44898</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E93" s="6">
         <v>130</v>
@@ -6569,13 +6656,13 @@
         <v>44899</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E94" s="6">
         <v>340</v>
@@ -6606,13 +6693,13 @@
         <v>44900</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E95" s="6">
         <v>215</v>
@@ -6643,13 +6730,13 @@
         <v>44900</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E96" s="6">
         <v>-110</v>
@@ -6664,15 +6751,15 @@
         <v>1.91</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>201</v>
+        <v>4</v>
       </c>
       <c r="J96" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.90999999999999992</v>
       </c>
       <c r="K96" s="11">
         <f t="shared" si="4"/>
-        <v>35.70000000000001</v>
+        <v>36.610000000000007</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -6680,13 +6767,13 @@
         <v>44900</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E97" s="6">
         <v>-110</v>
@@ -6709,7 +6796,7 @@
       </c>
       <c r="K97" s="11">
         <f t="shared" si="4"/>
-        <v>33.70000000000001</v>
+        <v>34.610000000000007</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -6717,13 +6804,13 @@
         <v>44900</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E98" s="6">
         <v>-230</v>
@@ -6746,7 +6833,7 @@
       </c>
       <c r="K98" s="11">
         <f t="shared" si="4"/>
-        <v>34.13000000000001</v>
+        <v>35.040000000000006</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -6754,13 +6841,13 @@
         <v>44901</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E99" s="6">
         <v>230</v>
@@ -6783,7 +6870,7 @@
       </c>
       <c r="K99" s="11">
         <f t="shared" si="4"/>
-        <v>36.430000000000007</v>
+        <v>37.340000000000003</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -6791,13 +6878,13 @@
         <v>44902</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E100" s="6">
         <v>150</v>
@@ -6820,7 +6907,7 @@
       </c>
       <c r="K100" s="11">
         <f t="shared" si="4"/>
-        <v>35.430000000000007</v>
+        <v>36.340000000000003</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -6828,13 +6915,13 @@
         <v>44902</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="E101" s="6">
         <v>-115</v>
@@ -6857,7 +6944,7 @@
       </c>
       <c r="K101" s="11">
         <f t="shared" si="4"/>
-        <v>36.300000000000004</v>
+        <v>37.21</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -6865,13 +6952,13 @@
         <v>44902</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E102" s="6">
         <v>-175</v>
@@ -6894,7 +6981,7 @@
       </c>
       <c r="K102" s="11">
         <f t="shared" si="4"/>
-        <v>37.440000000000005</v>
+        <v>38.35</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -6902,13 +6989,13 @@
         <v>44902</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E103" s="6">
         <v>125</v>
@@ -6931,7 +7018,7 @@
       </c>
       <c r="K103" s="11">
         <f t="shared" si="4"/>
-        <v>36.440000000000005</v>
+        <v>37.35</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -6939,13 +7026,13 @@
         <v>44902</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E104" s="6">
         <v>800</v>
@@ -6968,7 +7055,7 @@
       </c>
       <c r="K104" s="11">
         <f t="shared" si="4"/>
-        <v>35.440000000000005</v>
+        <v>36.35</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -6976,13 +7063,13 @@
         <v>44903</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E105" s="6">
         <v>-125</v>
@@ -7005,7 +7092,7 @@
       </c>
       <c r="K105" s="11">
         <f t="shared" si="4"/>
-        <v>34.440000000000005</v>
+        <v>35.35</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -7013,13 +7100,13 @@
         <v>44903</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E106" s="6">
         <v>255</v>
@@ -7042,7 +7129,7 @@
       </c>
       <c r="K106" s="11">
         <f t="shared" si="4"/>
-        <v>33.440000000000005</v>
+        <v>34.35</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -7050,13 +7137,13 @@
         <v>44903</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E107" s="6">
         <v>120</v>
@@ -7079,7 +7166,7 @@
       </c>
       <c r="K107" s="11">
         <f t="shared" si="4"/>
-        <v>34.640000000000008</v>
+        <v>35.550000000000004</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -7087,13 +7174,13 @@
         <v>44904</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E108" s="6">
         <v>160</v>
@@ -7111,12 +7198,12 @@
         <v>5</v>
       </c>
       <c r="J108" s="11">
-        <f t="shared" ref="J108:J112" si="5">IF(I108="Pending", 0,IF(I108="Win",H108-G108,-1*G108))</f>
+        <f t="shared" ref="J108:J116" si="5">IF(I108="Pending", 0,IF(I108="Win",H108-G108,-1*G108))</f>
         <v>-2</v>
       </c>
       <c r="K108" s="11">
         <f t="shared" si="4"/>
-        <v>32.640000000000008</v>
+        <v>33.550000000000004</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -7124,13 +7211,13 @@
         <v>44904</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E109" s="6">
         <v>130</v>
@@ -7153,7 +7240,7 @@
       </c>
       <c r="K109" s="11">
         <f t="shared" si="4"/>
-        <v>31.640000000000008</v>
+        <v>32.550000000000004</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -7161,13 +7248,13 @@
         <v>44904</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E110" s="6">
         <v>-135</v>
@@ -7190,7 +7277,7 @@
       </c>
       <c r="K110" s="11">
         <f t="shared" si="4"/>
-        <v>29.640000000000008</v>
+        <v>30.550000000000004</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -7198,13 +7285,13 @@
         <v>44905</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E111" s="6">
         <v>125</v>
@@ -7227,7 +7314,7 @@
       </c>
       <c r="K111" s="11">
         <f t="shared" si="4"/>
-        <v>30.890000000000008</v>
+        <v>31.800000000000004</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
@@ -7235,19 +7322,19 @@
         <v>44906</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E112" s="6">
         <v>170</v>
       </c>
       <c r="F112" s="6">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="G112" s="11">
         <v>1</v>
@@ -7256,133 +7343,349 @@
         <v>2.7</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>201</v>
+        <v>5</v>
       </c>
       <c r="J112" s="11">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K112" s="11">
         <f t="shared" si="4"/>
-        <v>30.890000000000008</v>
+        <v>30.800000000000004</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="6"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="8"/>
-      <c r="J113" s="11"/>
-      <c r="K113" s="11"/>
+      <c r="A113" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E113" s="6">
+        <v>135</v>
+      </c>
+      <c r="F113" s="6">
+        <v>130</v>
+      </c>
+      <c r="G113" s="11">
+        <v>1</v>
+      </c>
+      <c r="H113" s="11">
+        <v>2.35</v>
+      </c>
+      <c r="I113" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J113" s="11">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K113" s="11">
+        <f t="shared" si="4"/>
+        <v>29.800000000000004</v>
+      </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="6"/>
-      <c r="F114" s="6"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="8"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
+      <c r="A114" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E114" s="6">
+        <v>130</v>
+      </c>
+      <c r="F114" s="6">
+        <v>115</v>
+      </c>
+      <c r="G114" s="11">
+        <v>1</v>
+      </c>
+      <c r="H114" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I114" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J114" s="11">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K114" s="11">
+        <f t="shared" si="4"/>
+        <v>28.800000000000004</v>
+      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="6"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="8"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="11"/>
+      <c r="A115" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E115" s="6">
+        <v>130</v>
+      </c>
+      <c r="F115" s="6">
+        <v>130</v>
+      </c>
+      <c r="G115" s="11">
+        <v>1</v>
+      </c>
+      <c r="H115" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I115" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J115" s="11">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K115" s="11">
+        <f t="shared" si="4"/>
+        <v>27.800000000000004</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
-      <c r="I116" s="8"/>
-      <c r="J116" s="11"/>
-      <c r="K116" s="11"/>
+      <c r="A116" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="E116" s="6">
+        <v>150</v>
+      </c>
+      <c r="F116" s="6">
+        <v>130</v>
+      </c>
+      <c r="G116" s="11">
+        <v>1</v>
+      </c>
+      <c r="H116" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="I116" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J116" s="11">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="K116" s="11">
+        <f t="shared" si="4"/>
+        <v>26.800000000000004</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="6"/>
-      <c r="F117" s="6"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="8"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
+      <c r="A117" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E117" s="6">
+        <v>145</v>
+      </c>
+      <c r="F117" s="6">
+        <v>140</v>
+      </c>
+      <c r="G117" s="11">
+        <v>1</v>
+      </c>
+      <c r="H117" s="11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I117" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J117" s="11">
+        <f t="shared" ref="J117:J121" si="6">IF(I117="Pending", 0,IF(I117="Win",H117-G117,-1*G117))</f>
+        <v>-1</v>
+      </c>
+      <c r="K117" s="11">
+        <f t="shared" ref="K117" si="7">K116+J117</f>
+        <v>25.800000000000004</v>
+      </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="6"/>
-      <c r="F118" s="6"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="8"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="11"/>
+      <c r="A118" s="7">
+        <v>44907</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E118" s="6">
+        <v>-110</v>
+      </c>
+      <c r="F118" s="6">
+        <v>-110</v>
+      </c>
+      <c r="G118" s="11">
+        <v>1</v>
+      </c>
+      <c r="H118" s="11">
+        <v>1.91</v>
+      </c>
+      <c r="I118" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J118" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K118" s="11">
+        <f t="shared" si="4"/>
+        <v>24.800000000000004</v>
+      </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="6"/>
-      <c r="F119" s="6"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="8"/>
-      <c r="J119" s="11"/>
-      <c r="K119" s="11"/>
+      <c r="A119" s="7">
+        <v>44908</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E119" s="6">
+        <v>170</v>
+      </c>
+      <c r="F119" s="6">
+        <v>170</v>
+      </c>
+      <c r="G119" s="11">
+        <v>1</v>
+      </c>
+      <c r="H119" s="11">
+        <v>2.7</v>
+      </c>
+      <c r="I119" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J119" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K119" s="11">
+        <f t="shared" si="4"/>
+        <v>23.800000000000004</v>
+      </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="11"/>
-      <c r="H120" s="11"/>
-      <c r="I120" s="8"/>
-      <c r="J120" s="11"/>
-      <c r="K120" s="11"/>
+      <c r="A120" s="7">
+        <v>44908</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E120" s="6">
+        <v>140</v>
+      </c>
+      <c r="F120" s="6">
+        <v>140</v>
+      </c>
+      <c r="G120" s="11">
+        <v>1</v>
+      </c>
+      <c r="H120" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="I120" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J120" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K120" s="11">
+        <f t="shared" si="4"/>
+        <v>22.800000000000004</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="8"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="11"/>
-      <c r="I121" s="8"/>
-      <c r="J121" s="11"/>
-      <c r="K121" s="11"/>
+      <c r="A121" s="7">
+        <v>44908</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E121" s="6">
+        <v>105</v>
+      </c>
+      <c r="F121" s="6">
+        <v>105</v>
+      </c>
+      <c r="G121" s="11">
+        <v>1</v>
+      </c>
+      <c r="H121" s="11">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I121" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J121" s="11">
+        <f t="shared" si="6"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="K121" s="11">
+        <f t="shared" si="4"/>
+        <v>23.850000000000005</v>
+      </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="8"/>

</xml_diff>

<commit_message>
updated class names for pinnacle scraper
</commit_message>
<xml_diff>
--- a/betting spreadsheet.xlsx
+++ b/betting spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Desktop\betting-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84BC3C-7087-402F-8108-9A5D9BC5F686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C99512-5186-43FF-BC79-75DA765927E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="262">
   <si>
     <t>Date</t>
   </si>
@@ -792,6 +792,39 @@
   </si>
   <si>
     <t>Toronto Maple Leafs -2.5</t>
+  </si>
+  <si>
+    <t>Troy vs UTSA</t>
+  </si>
+  <si>
+    <t>UTSA</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Stony Brook vs Wagner</t>
+  </si>
+  <si>
+    <t>Stony Brook</t>
+  </si>
+  <si>
+    <t>Dallas Stars vs Carolina Hurricanes</t>
+  </si>
+  <si>
+    <t>Dallas Stars +1.5</t>
+  </si>
+  <si>
+    <t>Clemson vs Tennessee</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Florida vs Oregon State</t>
+  </si>
+  <si>
+    <t>Florida</t>
   </si>
 </sst>
 </file>
@@ -1438,6 +1471,21 @@
                 </c:pt>
                 <c:pt idx="119">
                   <c:v>23.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>22.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>21.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>21.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>21.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>21.850000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3180,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9706E5D-ABEE-4E65-AA0D-26913405A8B0}">
   <dimension ref="A1:M158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L121" sqref="L121"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,7 +3325,7 @@
       </c>
       <c r="M2" s="13">
         <f>SUM(J2:J130)</f>
-        <v>23.850000000000005</v>
+        <v>21.850000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5612,7 +5660,7 @@
         <v>-1</v>
       </c>
       <c r="K65" s="11">
-        <f t="shared" ref="K65:K121" si="4">K64+J65</f>
+        <f t="shared" ref="K65:K126" si="4">K64+J65</f>
         <v>46.630000000000017</v>
       </c>
     </row>
@@ -7531,7 +7579,7 @@
         <v>5</v>
       </c>
       <c r="J117" s="11">
-        <f t="shared" ref="J117:J121" si="6">IF(I117="Pending", 0,IF(I117="Win",H117-G117,-1*G117))</f>
+        <f t="shared" ref="J117:J126" si="6">IF(I117="Pending", 0,IF(I117="Win",H117-G117,-1*G117))</f>
         <v>-1</v>
       </c>
       <c r="K117" s="11">
@@ -7688,69 +7736,189 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="6"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
-      <c r="I122" s="8"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="11"/>
+      <c r="A122" s="7">
+        <v>44909</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E122" s="6">
+        <v>105</v>
+      </c>
+      <c r="F122" s="6">
+        <v>105</v>
+      </c>
+      <c r="G122" s="11">
+        <v>1</v>
+      </c>
+      <c r="H122" s="11">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I122" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J122" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K122" s="11">
+        <f t="shared" si="4"/>
+        <v>22.850000000000005</v>
+      </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="6"/>
-      <c r="F123" s="6"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="8"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="11"/>
+      <c r="A123" s="7">
+        <v>44910</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E123" s="6">
+        <v>230</v>
+      </c>
+      <c r="F123" s="6">
+        <v>240</v>
+      </c>
+      <c r="G123" s="11">
+        <v>1</v>
+      </c>
+      <c r="H123" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="I123" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J123" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K123" s="11">
+        <f t="shared" si="4"/>
+        <v>21.850000000000005</v>
+      </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="8"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="11"/>
-      <c r="K124" s="11"/>
+      <c r="A124" s="7">
+        <v>44911</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E124" s="6">
+        <v>-175</v>
+      </c>
+      <c r="F124" s="6">
+        <v>-175</v>
+      </c>
+      <c r="G124" s="11">
+        <v>1</v>
+      </c>
+      <c r="H124" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="I124" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J124" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K124" s="11">
+        <f t="shared" si="4"/>
+        <v>21.850000000000005</v>
+      </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="8"/>
-      <c r="B125" s="8"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
-      <c r="I125" s="8"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="11"/>
+      <c r="A125" s="7">
+        <v>44911</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E125" s="6">
+        <v>215</v>
+      </c>
+      <c r="F125" s="6">
+        <v>215</v>
+      </c>
+      <c r="G125" s="11">
+        <v>1</v>
+      </c>
+      <c r="H125" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I125" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J125" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K125" s="11">
+        <f t="shared" si="4"/>
+        <v>21.850000000000005</v>
+      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="8"/>
-      <c r="B126" s="8"/>
-      <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="11"/>
-      <c r="I126" s="8"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="11"/>
+      <c r="A126" s="7">
+        <v>44912</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E126" s="6">
+        <v>260</v>
+      </c>
+      <c r="F126" s="6">
+        <v>260</v>
+      </c>
+      <c r="G126" s="11">
+        <v>1</v>
+      </c>
+      <c r="H126" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="I126" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J126" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K126" s="11">
+        <f t="shared" si="4"/>
+        <v>21.850000000000005</v>
+      </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>

</xml_diff>

<commit_message>
EPL and Euroleague implementation
</commit_message>
<xml_diff>
--- a/betting spreadsheet.xlsx
+++ b/betting spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Desktop\betting-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C99512-5186-43FF-BC79-75DA765927E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1DDC25-CC69-4127-9EB0-26CDBABD23CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$130</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$174</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="358">
   <si>
     <t>Date</t>
   </si>
@@ -770,12 +770,6 @@
     <t>UC San Diego +3.5</t>
   </si>
   <si>
-    <t>Los Angeles Rams vs Green Bay Packers</t>
-  </si>
-  <si>
-    <t>Los Angeles Rams +7.5</t>
-  </si>
-  <si>
     <t>MD Baltimore County vs Loyola Maryland</t>
   </si>
   <si>
@@ -825,6 +819,300 @@
   </si>
   <si>
     <t>Florida</t>
+  </si>
+  <si>
+    <t>Florida +7.5</t>
+  </si>
+  <si>
+    <t>Tampa Bay Lightning vs Montreal Canadiens</t>
+  </si>
+  <si>
+    <t>BYU vs SMU</t>
+  </si>
+  <si>
+    <t>BYU</t>
+  </si>
+  <si>
+    <t>UCLA vs Kentucky</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>San Jose State vs Pacific</t>
+  </si>
+  <si>
+    <t>San Jose State</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers vs Carolina Panthers</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers +4.5</t>
+  </si>
+  <si>
+    <t>Southern vs UAB</t>
+  </si>
+  <si>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>Hampton vs Texas Southern</t>
+  </si>
+  <si>
+    <t>Texas Southern</t>
+  </si>
+  <si>
+    <t>Iona vs New Mexico</t>
+  </si>
+  <si>
+    <t>New Mexico -5.5</t>
+  </si>
+  <si>
+    <t>San Diego vs Arizona State</t>
+  </si>
+  <si>
+    <t>San Diego +9.0</t>
+  </si>
+  <si>
+    <t>Over 143.5</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>Connecticut vs Marshall</t>
+  </si>
+  <si>
+    <t>Marshall -12.5</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers vs Arizona Cardinals</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>Toledo vs Liberty</t>
+  </si>
+  <si>
+    <t>Maine vs Akron</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Buffalo Sabres vs Vegas Golden Knights</t>
+  </si>
+  <si>
+    <t>Vegas Golden Knights -2.5</t>
+  </si>
+  <si>
+    <t>Utah Jazz vs Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Detroit Pistons -1.0</t>
+  </si>
+  <si>
+    <t>New York Islanders vs Colorado Avalanche</t>
+  </si>
+  <si>
+    <t>Colorado Avalanche -2.5</t>
+  </si>
+  <si>
+    <t>Wofford vs Texas A&amp;M</t>
+  </si>
+  <si>
+    <t>Under 144.0</t>
+  </si>
+  <si>
+    <t>Under 137.5</t>
+  </si>
+  <si>
+    <t>Washington Wizards vs Phoenix Suns</t>
+  </si>
+  <si>
+    <t>Washington Wizards</t>
+  </si>
+  <si>
+    <t>Golden State Warriors vs New York Knicks</t>
+  </si>
+  <si>
+    <t>Under 224.0</t>
+  </si>
+  <si>
+    <t>Under 138.0</t>
+  </si>
+  <si>
+    <t>Montreal Canadiens vs Colorado Avalanche</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers vs Sacramento Kings</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks vs Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Over 240.0</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks -1.5</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars vs New York Jets</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers vs Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder -1.0</t>
+  </si>
+  <si>
+    <t>Kent State vs New Mexico State</t>
+  </si>
+  <si>
+    <t>UL Lafayette vs Texas</t>
+  </si>
+  <si>
+    <t>Under 142.0</t>
+  </si>
+  <si>
+    <t>Over 37.5</t>
+  </si>
+  <si>
+    <t>Philadelphia Flyers vs Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>Iona vs SMU</t>
+  </si>
+  <si>
+    <t>East Carolina vs Coastal Carolina</t>
+  </si>
+  <si>
+    <t>Over 62.5</t>
+  </si>
+  <si>
+    <t>Mississippi State vs Illinois</t>
+  </si>
+  <si>
+    <t>Mississippi State -2.5</t>
+  </si>
+  <si>
+    <t>Kansas vs Arkansas</t>
+  </si>
+  <si>
+    <t>Kansas +5.0</t>
+  </si>
+  <si>
+    <t>Butler vs Creighton</t>
+  </si>
+  <si>
+    <t>Creighton -10.0</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers -6.5</t>
+  </si>
+  <si>
+    <t>Kansas +4.0</t>
+  </si>
+  <si>
+    <t>Indiana Pacers vs Miami Heat</t>
+  </si>
+  <si>
+    <t>St. Louis Blues vs Vegas Golden Knights</t>
+  </si>
+  <si>
+    <t>Houston Texans vs Tennessee Titans</t>
+  </si>
+  <si>
+    <t>Tennessee Titans -3.5</t>
+  </si>
+  <si>
+    <t>Buffalo Bills vs Chicago Bears</t>
+  </si>
+  <si>
+    <t>Under 42.5</t>
+  </si>
+  <si>
+    <t>Iona vs Pepperdine</t>
+  </si>
+  <si>
+    <t>Under 147.5</t>
+  </si>
+  <si>
+    <t>Mississippi State -1.5</t>
+  </si>
+  <si>
+    <t>Maryland vs NC State</t>
+  </si>
+  <si>
+    <t>Under 46.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers vs Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>Pittsburgh Penguins vs New York Islanders</t>
+  </si>
+  <si>
+    <t>Pittsburgh Penguins</t>
+  </si>
+  <si>
+    <t>San Jose Sharks vs Vancouver Canucks</t>
+  </si>
+  <si>
+    <t>Iowa vs Kentucky</t>
+  </si>
+  <si>
+    <t>Under 29.0</t>
+  </si>
+  <si>
+    <t>Carolina Panthers vs Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>Denver Broncos vs Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>Chicago Bears vs Detroit Lions</t>
+  </si>
+  <si>
+    <t>Chicago Bears</t>
+  </si>
+  <si>
+    <t>Chicago Blackhawks vs Carolina Huricanes</t>
+  </si>
+  <si>
+    <t>Carolina Hurricanes -2.5</t>
+  </si>
+  <si>
+    <t>Wichita State vs Central Florida</t>
+  </si>
+  <si>
+    <t>Wichita State +4.0</t>
+  </si>
+  <si>
+    <t>Davidson vs Fordham</t>
+  </si>
+  <si>
+    <t>Under 139.0</t>
+  </si>
+  <si>
+    <t>Boise State vs Nevada</t>
+  </si>
+  <si>
+    <t>Boise State</t>
+  </si>
+  <si>
+    <t>Zalgiris vs AS Monaco</t>
+  </si>
+  <si>
+    <t>Zalgiris +7.0</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1396,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$130</c:f>
+              <c:f>Sheet1!$K$2:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="129"/>
+                <c:ptCount val="173"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -1467,7 +1755,7 @@
                   <c:v>23.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>22.800000000000004</c:v>
+                  <c:v>24.850000000000005</c:v>
                 </c:pt>
                 <c:pt idx="119">
                   <c:v>23.850000000000005</c:v>
@@ -1476,16 +1764,160 @@
                   <c:v>22.850000000000005</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>21.850000000000005</c:v>
+                  <c:v>23.420000000000005</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>21.850000000000005</c:v>
+                  <c:v>23.420000000000005</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>21.850000000000005</c:v>
+                  <c:v>22.420000000000005</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>21.850000000000005</c:v>
+                  <c:v>21.420000000000005</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>20.420000000000005</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>22.070000000000004</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>22.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>21.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>22.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>21.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>22.420000000000005</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>23.820000000000004</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>22.820000000000004</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>24.070000000000004</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>24.740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>25.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>26.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>25.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>24.910000000000004</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>23.910000000000004</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>22.910000000000004</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>22.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>23.280000000000005</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>24.530000000000005</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>25.730000000000004</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>26.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>25.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>24.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>25.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>24.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>23.930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>25.380000000000003</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>25.980000000000004</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>26.630000000000003</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>27.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>27.870000000000005</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>28.820000000000004</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>28.820000000000004</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>29.490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>30.14</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>29.14</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>29.88</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>30.96</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>30.46</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>29.96</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>29.46</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>32.06</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>32.06</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>32.06</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>31.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>31.060000000000002</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>30.560000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1693,7 +2125,7 @@
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="waterfall" uniqueId="{AEDEC493-1E32-4D36-99EF-67EAF86BF7E1}">
+        <cx:series layoutId="waterfall" uniqueId="{CAA0484D-3C77-403A-9915-3F945E5D3CB7}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:subtotals/>
@@ -3226,10 +3658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9706E5D-ABEE-4E65-AA0D-26913405A8B0}">
-  <dimension ref="A1:M158"/>
+  <dimension ref="A1:M199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L124" sqref="L124"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I184" sqref="I184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3324,8 +3756,8 @@
         <v>1.5</v>
       </c>
       <c r="M2" s="13">
-        <f>SUM(J2:J130)</f>
-        <v>21.850000000000005</v>
+        <f>SUM(J2:J190)</f>
+        <v>28.860000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5660,7 +6092,7 @@
         <v>-1</v>
       </c>
       <c r="K65" s="11">
-        <f t="shared" ref="K65:K126" si="4">K64+J65</f>
+        <f t="shared" ref="K65:K128" si="4">K64+J65</f>
         <v>46.630000000000017</v>
       </c>
     </row>
@@ -7579,7 +8011,7 @@
         <v>5</v>
       </c>
       <c r="J117" s="11">
-        <f t="shared" ref="J117:J126" si="6">IF(I117="Pending", 0,IF(I117="Win",H117-G117,-1*G117))</f>
+        <f t="shared" ref="J117:J136" si="6">IF(I117="Pending", 0,IF(I117="Win",H117-G117,-1*G117))</f>
         <v>-1</v>
       </c>
       <c r="K117" s="11">
@@ -7589,28 +8021,28 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
-        <v>44907</v>
+        <v>44908</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>243</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D118" s="8" t="s">
         <v>244</v>
       </c>
       <c r="E118" s="6">
-        <v>-110</v>
+        <v>170</v>
       </c>
       <c r="F118" s="6">
-        <v>-110</v>
+        <v>170</v>
       </c>
       <c r="G118" s="11">
         <v>1</v>
       </c>
       <c r="H118" s="11">
-        <v>1.91</v>
+        <v>2.7</v>
       </c>
       <c r="I118" s="8" t="s">
         <v>5</v>
@@ -7632,22 +8064,22 @@
         <v>245</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>50</v>
+        <v>205</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>246</v>
       </c>
       <c r="E119" s="6">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="F119" s="6">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="G119" s="11">
         <v>1</v>
       </c>
       <c r="H119" s="11">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="I119" s="8" t="s">
         <v>5</v>
@@ -7675,38 +8107,38 @@
         <v>248</v>
       </c>
       <c r="E120" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="F120" s="6">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="G120" s="11">
         <v>1</v>
       </c>
       <c r="H120" s="11">
-        <v>2.4</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J120" s="11">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>1.0499999999999998</v>
       </c>
       <c r="K120" s="11">
         <f t="shared" si="4"/>
-        <v>22.800000000000004</v>
+        <v>24.850000000000005</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
-        <v>44908</v>
+        <v>44909</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>249</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>205</v>
+        <v>50</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>250</v>
@@ -7724,11 +8156,11 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J121" s="11">
         <f t="shared" si="6"/>
-        <v>1.0499999999999998</v>
+        <v>-1</v>
       </c>
       <c r="K121" s="11">
         <f t="shared" si="4"/>
@@ -7737,28 +8169,28 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
-        <v>44909</v>
+        <v>44910</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E122" s="6">
-        <v>105</v>
+        <v>230</v>
       </c>
       <c r="F122" s="6">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="G122" s="11">
         <v>1</v>
       </c>
       <c r="H122" s="11">
-        <v>2.0499999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="I122" s="8" t="s">
         <v>5</v>
@@ -7774,39 +8206,39 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
-        <v>44910</v>
+        <v>44911</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>254</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>255</v>
       </c>
       <c r="E123" s="6">
-        <v>230</v>
+        <v>-175</v>
       </c>
       <c r="F123" s="6">
-        <v>240</v>
+        <v>-195</v>
       </c>
       <c r="G123" s="11">
         <v>1</v>
       </c>
       <c r="H123" s="11">
-        <v>3.3</v>
+        <v>1.57</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J123" s="11">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="K123" s="11">
         <f t="shared" si="4"/>
-        <v>21.850000000000005</v>
+        <v>23.420000000000005</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -7817,25 +8249,25 @@
         <v>256</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>257</v>
       </c>
       <c r="E124" s="6">
-        <v>-175</v>
+        <v>215</v>
       </c>
       <c r="F124" s="6">
-        <v>-175</v>
+        <v>175</v>
       </c>
       <c r="G124" s="11">
         <v>1</v>
       </c>
       <c r="H124" s="11">
-        <v>1.57</v>
+        <v>3.15</v>
       </c>
       <c r="I124" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J124" s="11">
         <f t="shared" si="6"/>
@@ -7843,12 +8275,12 @@
       </c>
       <c r="K124" s="11">
         <f t="shared" si="4"/>
-        <v>21.850000000000005</v>
+        <v>23.420000000000005</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
-        <v>44911</v>
+        <v>44912</v>
       </c>
       <c r="B125" s="8" t="s">
         <v>258</v>
@@ -7860,27 +8292,27 @@
         <v>259</v>
       </c>
       <c r="E125" s="6">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="F125" s="6">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="G125" s="11">
         <v>1</v>
       </c>
       <c r="H125" s="11">
-        <v>3.15</v>
+        <v>3.6</v>
       </c>
       <c r="I125" s="8" t="s">
-        <v>253</v>
+        <v>5</v>
       </c>
       <c r="J125" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K125" s="11">
         <f t="shared" si="4"/>
-        <v>21.850000000000005</v>
+        <v>22.420000000000005</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
@@ -7888,453 +8320,2387 @@
         <v>44912</v>
       </c>
       <c r="B126" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="C126" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>261</v>
-      </c>
       <c r="E126" s="6">
-        <v>260</v>
+        <v>100</v>
       </c>
       <c r="F126" s="6">
-        <v>260</v>
+        <v>-115</v>
       </c>
       <c r="G126" s="11">
         <v>1</v>
       </c>
       <c r="H126" s="11">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="I126" s="8" t="s">
-        <v>253</v>
+        <v>5</v>
       </c>
       <c r="J126" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K126" s="11">
         <f t="shared" si="4"/>
-        <v>21.850000000000005</v>
+        <v>21.420000000000005</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A127" s="8"/>
-      <c r="B127" s="8"/>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="6"/>
-      <c r="F127" s="6"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
-      <c r="I127" s="8"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="11"/>
+      <c r="A127" s="7">
+        <v>44912</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E127" s="6">
+        <v>135</v>
+      </c>
+      <c r="F127" s="6">
+        <v>135</v>
+      </c>
+      <c r="G127" s="11">
+        <v>1</v>
+      </c>
+      <c r="H127" s="11">
+        <v>2.35</v>
+      </c>
+      <c r="I127" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J127" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K127" s="11">
+        <f t="shared" si="4"/>
+        <v>20.420000000000005</v>
+      </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
-      <c r="B128" s="8"/>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="11"/>
-      <c r="I128" s="8"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="11"/>
+      <c r="A128" s="7">
+        <v>44912</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E128" s="6">
+        <v>165</v>
+      </c>
+      <c r="F128" s="6">
+        <v>165</v>
+      </c>
+      <c r="G128" s="11">
+        <v>1</v>
+      </c>
+      <c r="H128" s="11">
+        <v>2.65</v>
+      </c>
+      <c r="I128" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J128" s="11">
+        <f t="shared" si="6"/>
+        <v>1.65</v>
+      </c>
+      <c r="K128" s="11">
+        <f t="shared" si="4"/>
+        <v>22.070000000000004</v>
+      </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="8"/>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="11"/>
-      <c r="H129" s="11"/>
-      <c r="I129" s="8"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="11"/>
+      <c r="A129" s="7">
+        <v>44912</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C129" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E129" s="6">
+        <v>-130</v>
+      </c>
+      <c r="F129" s="6">
+        <v>-130</v>
+      </c>
+      <c r="G129" s="11">
+        <v>1</v>
+      </c>
+      <c r="H129" s="11">
+        <v>1.77</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J129" s="11">
+        <f t="shared" si="6"/>
+        <v>0.77</v>
+      </c>
+      <c r="K129" s="11">
+        <f t="shared" ref="K129:K192" si="8">K128+J129</f>
+        <v>22.840000000000003</v>
+      </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="8"/>
-      <c r="B130" s="8"/>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="6"/>
-      <c r="G130" s="11"/>
-      <c r="H130" s="11"/>
-      <c r="I130" s="8"/>
-      <c r="J130" s="11"/>
-      <c r="K130" s="11"/>
+      <c r="A130" s="7">
+        <v>44912</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E130" s="6">
+        <v>125</v>
+      </c>
+      <c r="F130" s="6">
+        <v>115</v>
+      </c>
+      <c r="G130" s="11">
+        <v>1</v>
+      </c>
+      <c r="H130" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="I130" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J130" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K130" s="11">
+        <f t="shared" si="8"/>
+        <v>21.840000000000003</v>
+      </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A131" s="8"/>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="6"/>
-      <c r="F131" s="6"/>
-      <c r="G131" s="11"/>
-      <c r="H131" s="11"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="11"/>
-      <c r="K131" s="11"/>
+      <c r="A131" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E131" s="6">
+        <v>-150</v>
+      </c>
+      <c r="F131" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G131" s="11">
+        <v>1</v>
+      </c>
+      <c r="H131" s="11">
+        <v>1.67</v>
+      </c>
+      <c r="I131" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J131" s="11">
+        <f t="shared" si="6"/>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="K131" s="11">
+        <f t="shared" si="8"/>
+        <v>22.510000000000005</v>
+      </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8"/>
-      <c r="C132" s="8"/>
-      <c r="D132" s="8"/>
-      <c r="E132" s="6"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="11"/>
-      <c r="H132" s="11"/>
-      <c r="I132" s="8"/>
-      <c r="J132" s="11"/>
-      <c r="K132" s="11"/>
+      <c r="A132" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E132" s="6">
+        <v>1200</v>
+      </c>
+      <c r="F132" s="6">
+        <v>1200</v>
+      </c>
+      <c r="G132" s="11">
+        <v>1</v>
+      </c>
+      <c r="H132" s="11">
+        <v>13</v>
+      </c>
+      <c r="I132" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J132" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K132" s="11">
+        <f t="shared" si="8"/>
+        <v>21.510000000000005</v>
+      </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="8"/>
-      <c r="B133" s="8"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="6"/>
-      <c r="F133" s="6"/>
-      <c r="G133" s="11"/>
-      <c r="H133" s="11"/>
-      <c r="I133" s="8"/>
-      <c r="J133" s="11"/>
-      <c r="K133" s="11"/>
+      <c r="A133" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D133" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E133" s="6">
+        <v>-220</v>
+      </c>
+      <c r="F133" s="6">
+        <v>-275</v>
+      </c>
+      <c r="G133" s="11">
+        <v>2</v>
+      </c>
+      <c r="H133" s="11">
+        <v>2.91</v>
+      </c>
+      <c r="I133" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J133" s="11">
+        <f t="shared" si="6"/>
+        <v>0.91000000000000014</v>
+      </c>
+      <c r="K133" s="11">
+        <f t="shared" si="8"/>
+        <v>22.420000000000005</v>
+      </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="8"/>
-      <c r="B134" s="8"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="6"/>
-      <c r="F134" s="6"/>
-      <c r="G134" s="11"/>
-      <c r="H134" s="11"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="11"/>
-      <c r="K134" s="11"/>
+      <c r="A134" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D134" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="E134" s="6">
+        <v>140</v>
+      </c>
+      <c r="F134" s="6">
+        <v>140</v>
+      </c>
+      <c r="G134" s="11">
+        <v>1</v>
+      </c>
+      <c r="H134" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="I134" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J134" s="11">
+        <f t="shared" si="6"/>
+        <v>1.4</v>
+      </c>
+      <c r="K134" s="11">
+        <f t="shared" si="8"/>
+        <v>23.820000000000004</v>
+      </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="8"/>
-      <c r="B135" s="8"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="6"/>
-      <c r="F135" s="6"/>
-      <c r="G135" s="11"/>
-      <c r="H135" s="11"/>
-      <c r="I135" s="8"/>
-      <c r="J135" s="11"/>
-      <c r="K135" s="11"/>
+      <c r="A135" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E135" s="6">
+        <v>135</v>
+      </c>
+      <c r="F135" s="6">
+        <v>115</v>
+      </c>
+      <c r="G135" s="11">
+        <v>1</v>
+      </c>
+      <c r="H135" s="11">
+        <v>2.35</v>
+      </c>
+      <c r="I135" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J135" s="11">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="K135" s="11">
+        <f t="shared" si="8"/>
+        <v>22.820000000000004</v>
+      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="8"/>
-      <c r="B136" s="8"/>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-      <c r="E136" s="6"/>
-      <c r="F136" s="6"/>
-      <c r="G136" s="11"/>
-      <c r="H136" s="11"/>
-      <c r="I136" s="8"/>
-      <c r="J136" s="11"/>
-      <c r="K136" s="11"/>
+      <c r="A136" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D136" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E136" s="6">
+        <v>125</v>
+      </c>
+      <c r="F136" s="6">
+        <v>125</v>
+      </c>
+      <c r="G136" s="11">
+        <v>1</v>
+      </c>
+      <c r="H136" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="I136" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J136" s="11">
+        <f t="shared" si="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="K136" s="11">
+        <f t="shared" si="8"/>
+        <v>24.070000000000004</v>
+      </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="8"/>
-      <c r="B137" s="8"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="6"/>
-      <c r="F137" s="6"/>
-      <c r="G137" s="11"/>
-      <c r="H137" s="11"/>
-      <c r="I137" s="8"/>
-      <c r="J137" s="11"/>
-      <c r="K137" s="11"/>
+      <c r="A137" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D137" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E137" s="6">
+        <v>-150</v>
+      </c>
+      <c r="F137" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G137" s="11">
+        <v>1</v>
+      </c>
+      <c r="H137" s="11">
+        <v>1.67</v>
+      </c>
+      <c r="I137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J137" s="11">
+        <f t="shared" ref="J137:J145" si="9">IF(I137="Pending", 0,IF(I137="Win",H137-G137,-1*G137))</f>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="K137" s="11">
+        <f t="shared" si="8"/>
+        <v>24.740000000000002</v>
+      </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A138" s="8"/>
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="6"/>
-      <c r="F138" s="6"/>
-      <c r="G138" s="11"/>
-      <c r="H138" s="11"/>
-      <c r="I138" s="8"/>
-      <c r="J138" s="11"/>
-      <c r="K138" s="11"/>
+      <c r="A138" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D138" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E138" s="6">
+        <v>110</v>
+      </c>
+      <c r="F138" s="6">
+        <v>-105</v>
+      </c>
+      <c r="G138" s="11">
+        <v>1</v>
+      </c>
+      <c r="H138" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="I138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J138" s="11">
+        <f t="shared" si="9"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K138" s="11">
+        <f t="shared" si="8"/>
+        <v>25.840000000000003</v>
+      </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="8"/>
-      <c r="B139" s="8"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="6"/>
-      <c r="F139" s="6"/>
-      <c r="G139" s="11"/>
-      <c r="H139" s="11"/>
-      <c r="I139" s="8"/>
-      <c r="J139" s="11"/>
-      <c r="K139" s="11"/>
+      <c r="A139" s="7">
+        <v>44913</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E139" s="6">
+        <v>-175</v>
+      </c>
+      <c r="F139" s="6">
+        <v>-400</v>
+      </c>
+      <c r="G139" s="11">
+        <v>1</v>
+      </c>
+      <c r="H139" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="I139" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J139" s="11">
+        <f t="shared" si="9"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="K139" s="11">
+        <f t="shared" si="8"/>
+        <v>26.410000000000004</v>
+      </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="8"/>
-      <c r="B140" s="8"/>
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
-      <c r="E140" s="6"/>
-      <c r="F140" s="6"/>
-      <c r="G140" s="11"/>
-      <c r="H140" s="11"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="11"/>
-      <c r="K140" s="11"/>
+      <c r="A140" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="E140" s="6">
+        <v>160</v>
+      </c>
+      <c r="F140" s="6">
+        <v>145</v>
+      </c>
+      <c r="G140" s="11">
+        <v>1</v>
+      </c>
+      <c r="H140" s="11">
+        <v>2.6</v>
+      </c>
+      <c r="I140" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J140" s="11">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="K140" s="11">
+        <f t="shared" si="8"/>
+        <v>25.410000000000004</v>
+      </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A141" s="8"/>
-      <c r="B141" s="8"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="6"/>
-      <c r="F141" s="6"/>
-      <c r="G141" s="11"/>
-      <c r="H141" s="11"/>
-      <c r="I141" s="8"/>
-      <c r="J141" s="11"/>
-      <c r="K141" s="11"/>
+      <c r="A141" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D141" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="E141" s="6">
+        <v>650</v>
+      </c>
+      <c r="F141" s="6">
+        <v>650</v>
+      </c>
+      <c r="G141" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H141" s="11">
+        <v>3.75</v>
+      </c>
+      <c r="I141" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J141" s="11">
+        <f t="shared" si="9"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K141" s="11">
+        <f t="shared" si="8"/>
+        <v>24.910000000000004</v>
+      </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A142" s="8"/>
-      <c r="B142" s="8"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="6"/>
-      <c r="F142" s="6"/>
-      <c r="G142" s="11"/>
-      <c r="H142" s="11"/>
-      <c r="I142" s="8"/>
-      <c r="J142" s="11"/>
-      <c r="K142" s="11"/>
+      <c r="A142" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D142" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E142" s="6">
+        <v>295</v>
+      </c>
+      <c r="F142" s="6">
+        <v>295</v>
+      </c>
+      <c r="G142" s="11">
+        <v>1</v>
+      </c>
+      <c r="H142" s="11">
+        <v>3.95</v>
+      </c>
+      <c r="I142" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J142" s="11">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="K142" s="11">
+        <f t="shared" si="8"/>
+        <v>23.910000000000004</v>
+      </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A143" s="8"/>
-      <c r="B143" s="8"/>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="6"/>
-      <c r="F143" s="6"/>
-      <c r="G143" s="11"/>
-      <c r="H143" s="11"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="11"/>
-      <c r="K143" s="11"/>
+      <c r="A143" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D143" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E143" s="6">
+        <v>145</v>
+      </c>
+      <c r="F143" s="6">
+        <v>115</v>
+      </c>
+      <c r="G143" s="11">
+        <v>1</v>
+      </c>
+      <c r="H143" s="11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I143" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J143" s="11">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="K143" s="11">
+        <f t="shared" si="8"/>
+        <v>22.910000000000004</v>
+      </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A144" s="8"/>
-      <c r="B144" s="8"/>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
-      <c r="G144" s="11"/>
-      <c r="H144" s="11"/>
-      <c r="I144" s="8"/>
-      <c r="J144" s="11"/>
-      <c r="K144" s="11"/>
+      <c r="A144" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D144" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E144" s="6">
+        <v>320</v>
+      </c>
+      <c r="F144" s="6">
+        <v>320</v>
+      </c>
+      <c r="G144" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H144" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="I144" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J144" s="11">
+        <f t="shared" si="9"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K144" s="11">
+        <f t="shared" si="8"/>
+        <v>22.410000000000004</v>
+      </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="8"/>
-      <c r="B145" s="8"/>
-      <c r="C145" s="8"/>
-      <c r="D145" s="8"/>
-      <c r="E145" s="6"/>
-      <c r="F145" s="6"/>
-      <c r="G145" s="11"/>
-      <c r="H145" s="11"/>
-      <c r="I145" s="8"/>
-      <c r="J145" s="11"/>
-      <c r="K145" s="11"/>
+      <c r="A145" s="7">
+        <v>44914</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D145" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E145" s="6">
+        <v>-115</v>
+      </c>
+      <c r="F145" s="6">
+        <v>-185</v>
+      </c>
+      <c r="G145" s="11">
+        <v>1</v>
+      </c>
+      <c r="H145" s="11">
+        <v>1.87</v>
+      </c>
+      <c r="I145" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J145" s="11">
+        <f t="shared" si="9"/>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="K145" s="11">
+        <f t="shared" si="8"/>
+        <v>23.280000000000005</v>
+      </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="8"/>
-      <c r="B146" s="8"/>
-      <c r="C146" s="8"/>
-      <c r="D146" s="8"/>
-      <c r="E146" s="6"/>
-      <c r="F146" s="6"/>
-      <c r="G146" s="11"/>
-      <c r="H146" s="11"/>
-      <c r="I146" s="8"/>
-      <c r="J146" s="11"/>
-      <c r="K146" s="11"/>
+      <c r="A146" s="7">
+        <v>44915</v>
+      </c>
+      <c r="B146" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E146" s="6">
+        <v>125</v>
+      </c>
+      <c r="F146" s="6">
+        <v>115</v>
+      </c>
+      <c r="G146" s="11">
+        <v>1</v>
+      </c>
+      <c r="H146" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="I146" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J146" s="11">
+        <f t="shared" ref="J146:J163" si="10">IF(I146="Pending", 0,IF(I146="Win",H146-G146,-1*G146))</f>
+        <v>1.25</v>
+      </c>
+      <c r="K146" s="11">
+        <f t="shared" si="8"/>
+        <v>24.530000000000005</v>
+      </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147" s="8"/>
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="6"/>
-      <c r="F147" s="6"/>
-      <c r="G147" s="11"/>
-      <c r="H147" s="11"/>
-      <c r="I147" s="8"/>
-      <c r="J147" s="11"/>
-      <c r="K147" s="11"/>
+      <c r="A147" s="7">
+        <v>44915</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E147" s="6">
+        <v>120</v>
+      </c>
+      <c r="F147" s="6">
+        <v>110</v>
+      </c>
+      <c r="G147" s="11">
+        <v>1</v>
+      </c>
+      <c r="H147" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I147" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J147" s="11">
+        <f t="shared" si="10"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="K147" s="11">
+        <f t="shared" si="8"/>
+        <v>25.730000000000004</v>
+      </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148" s="8"/>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
-      <c r="E148" s="6"/>
-      <c r="F148" s="6"/>
-      <c r="G148" s="11"/>
-      <c r="H148" s="11"/>
-      <c r="I148" s="8"/>
-      <c r="J148" s="11"/>
-      <c r="K148" s="11"/>
+      <c r="A148" s="7">
+        <v>44915</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E148" s="6">
+        <v>240</v>
+      </c>
+      <c r="F148" s="6">
+        <v>240</v>
+      </c>
+      <c r="G148" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H148" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="I148" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J148" s="11">
+        <f t="shared" si="10"/>
+        <v>1.2</v>
+      </c>
+      <c r="K148" s="11">
+        <f t="shared" si="8"/>
+        <v>26.930000000000003</v>
+      </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="6"/>
-      <c r="F149" s="6"/>
-      <c r="G149" s="11"/>
-      <c r="H149" s="11"/>
-      <c r="I149" s="8"/>
-      <c r="J149" s="11"/>
-      <c r="K149" s="11"/>
+      <c r="A149" s="7">
+        <v>44915</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E149" s="6">
+        <v>-135</v>
+      </c>
+      <c r="F149" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G149" s="11">
+        <v>1</v>
+      </c>
+      <c r="H149" s="11">
+        <v>1.74</v>
+      </c>
+      <c r="I149" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J149" s="11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="K149" s="11">
+        <f t="shared" si="8"/>
+        <v>25.930000000000003</v>
+      </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150" s="8"/>
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="6"/>
-      <c r="G150" s="11"/>
-      <c r="H150" s="11"/>
-      <c r="I150" s="8"/>
-      <c r="J150" s="11"/>
-      <c r="K150" s="11"/>
+      <c r="A150" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E150" s="6">
+        <v>185</v>
+      </c>
+      <c r="F150" s="6">
+        <v>185</v>
+      </c>
+      <c r="G150" s="11">
+        <v>1</v>
+      </c>
+      <c r="H150" s="11">
+        <v>2.85</v>
+      </c>
+      <c r="I150" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J150" s="11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="K150" s="11">
+        <f t="shared" si="8"/>
+        <v>24.930000000000003</v>
+      </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151" s="8"/>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="6"/>
-      <c r="F151" s="6"/>
-      <c r="G151" s="11"/>
-      <c r="H151" s="11"/>
-      <c r="I151" s="8"/>
-      <c r="J151" s="11"/>
-      <c r="K151" s="11"/>
+      <c r="A151" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D151" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E151" s="6">
+        <v>100</v>
+      </c>
+      <c r="F151" s="6">
+        <v>100</v>
+      </c>
+      <c r="G151" s="11">
+        <v>1</v>
+      </c>
+      <c r="H151" s="11">
+        <v>2</v>
+      </c>
+      <c r="I151" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J151" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K151" s="11">
+        <f t="shared" si="8"/>
+        <v>25.930000000000003</v>
+      </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A152" s="8"/>
-      <c r="B152" s="8"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
-      <c r="E152" s="6"/>
-      <c r="F152" s="6"/>
-      <c r="G152" s="11"/>
-      <c r="H152" s="11"/>
-      <c r="I152" s="8"/>
-      <c r="J152" s="11"/>
-      <c r="K152" s="11"/>
+      <c r="A152" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E152" s="6">
+        <v>125</v>
+      </c>
+      <c r="F152" s="6">
+        <v>130</v>
+      </c>
+      <c r="G152" s="11">
+        <v>1</v>
+      </c>
+      <c r="H152" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="I152" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J152" s="11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="K152" s="11">
+        <f t="shared" si="8"/>
+        <v>24.930000000000003</v>
+      </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153" s="8"/>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="6"/>
-      <c r="G153" s="11"/>
-      <c r="H153" s="11"/>
-      <c r="I153" s="8"/>
-      <c r="J153" s="11"/>
-      <c r="K153" s="11"/>
+      <c r="A153" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E153" s="6">
+        <v>110</v>
+      </c>
+      <c r="F153" s="6">
+        <v>105</v>
+      </c>
+      <c r="G153" s="11">
+        <v>1</v>
+      </c>
+      <c r="H153" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="I153" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J153" s="11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="K153" s="11">
+        <f t="shared" si="8"/>
+        <v>23.930000000000003</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="6"/>
-      <c r="F154" s="6"/>
-      <c r="G154" s="11"/>
-      <c r="H154" s="11"/>
-      <c r="I154" s="8"/>
-      <c r="J154" s="11"/>
-      <c r="K154" s="11"/>
+      <c r="A154" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D154" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E154" s="6">
+        <v>145</v>
+      </c>
+      <c r="F154" s="6">
+        <v>145</v>
+      </c>
+      <c r="G154" s="11">
+        <v>1</v>
+      </c>
+      <c r="H154" s="11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I154" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J154" s="11">
+        <f t="shared" si="10"/>
+        <v>1.4500000000000002</v>
+      </c>
+      <c r="K154" s="11">
+        <f t="shared" si="8"/>
+        <v>25.380000000000003</v>
+      </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-      <c r="E155" s="6"/>
-      <c r="F155" s="6"/>
-      <c r="G155" s="11"/>
-      <c r="H155" s="11"/>
-      <c r="I155" s="8"/>
-      <c r="J155" s="11"/>
-      <c r="K155" s="11"/>
+      <c r="A155" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E155" s="6">
+        <v>120</v>
+      </c>
+      <c r="F155" s="6">
+        <v>120</v>
+      </c>
+      <c r="G155" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H155" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I155" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J155" s="11">
+        <f t="shared" si="10"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="K155" s="11">
+        <f t="shared" si="8"/>
+        <v>25.980000000000004</v>
+      </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
-      <c r="G156" s="11"/>
-      <c r="H156" s="11"/>
-      <c r="I156" s="8"/>
-      <c r="J156" s="11"/>
-      <c r="K156" s="11"/>
+      <c r="A156" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E156" s="6">
+        <v>130</v>
+      </c>
+      <c r="F156" s="6">
+        <v>130</v>
+      </c>
+      <c r="G156" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H156" s="11">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I156" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J156" s="11">
+        <f t="shared" si="10"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="K156" s="11">
+        <f t="shared" si="8"/>
+        <v>26.630000000000003</v>
+      </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157" s="8"/>
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="E157" s="6"/>
-      <c r="F157" s="6"/>
-      <c r="G157" s="11"/>
-      <c r="H157" s="11"/>
-      <c r="I157" s="8"/>
-      <c r="J157" s="11"/>
-      <c r="K157" s="11"/>
+      <c r="A157" s="7">
+        <v>44916</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D157" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E157" s="6">
+        <v>-270</v>
+      </c>
+      <c r="F157" s="6">
+        <v>-270</v>
+      </c>
+      <c r="G157" s="11">
+        <v>1</v>
+      </c>
+      <c r="H157" s="11">
+        <v>1.37</v>
+      </c>
+      <c r="I157" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J157" s="11">
+        <f t="shared" si="10"/>
+        <v>0.37000000000000011</v>
+      </c>
+      <c r="K157" s="11">
+        <f t="shared" si="8"/>
+        <v>27.000000000000004</v>
+      </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158" s="8"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="E158" s="6"/>
-      <c r="F158" s="6"/>
-      <c r="G158" s="11"/>
-      <c r="H158" s="11"/>
-      <c r="I158" s="8"/>
-      <c r="J158" s="11"/>
-      <c r="K158" s="11"/>
+      <c r="A158" s="7">
+        <v>44917</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E158" s="6">
+        <v>-115</v>
+      </c>
+      <c r="F158" s="6">
+        <v>-115</v>
+      </c>
+      <c r="G158" s="11">
+        <v>1</v>
+      </c>
+      <c r="H158" s="11">
+        <v>1.87</v>
+      </c>
+      <c r="I158" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J158" s="11">
+        <f t="shared" si="10"/>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="K158" s="11">
+        <f t="shared" si="8"/>
+        <v>27.870000000000005</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" s="7">
+        <v>44917</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E159" s="6">
+        <v>-105</v>
+      </c>
+      <c r="F159" s="6">
+        <v>-105</v>
+      </c>
+      <c r="G159" s="11">
+        <v>1</v>
+      </c>
+      <c r="H159" s="11">
+        <v>1.95</v>
+      </c>
+      <c r="I159" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J159" s="11">
+        <f t="shared" si="10"/>
+        <v>0.95</v>
+      </c>
+      <c r="K159" s="11">
+        <f t="shared" si="8"/>
+        <v>28.820000000000004</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" s="7">
+        <v>44917</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="E160" s="6">
+        <v>120</v>
+      </c>
+      <c r="F160" s="6">
+        <v>115</v>
+      </c>
+      <c r="G160" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H160" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I160" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J160" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K160" s="11">
+        <f t="shared" si="8"/>
+        <v>28.820000000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161" s="7">
+        <v>44917</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D161" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="E161" s="6">
+        <v>-150</v>
+      </c>
+      <c r="F161" s="6">
+        <v>-160</v>
+      </c>
+      <c r="G161" s="11">
+        <v>1</v>
+      </c>
+      <c r="H161" s="11">
+        <v>1.67</v>
+      </c>
+      <c r="I161" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J161" s="11">
+        <f t="shared" si="10"/>
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="K161" s="11">
+        <f t="shared" si="8"/>
+        <v>29.490000000000002</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162" s="7">
+        <v>44917</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="E162" s="6">
+        <v>130</v>
+      </c>
+      <c r="F162" s="6">
+        <v>130</v>
+      </c>
+      <c r="G162" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H162" s="11">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J162" s="11">
+        <f t="shared" si="10"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="K162" s="11">
+        <f t="shared" si="8"/>
+        <v>30.14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E163" s="6">
+        <v>-135</v>
+      </c>
+      <c r="F163" s="6">
+        <v>-135</v>
+      </c>
+      <c r="G163" s="11">
+        <v>1</v>
+      </c>
+      <c r="H163" s="11">
+        <v>1.74</v>
+      </c>
+      <c r="I163" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J163" s="11">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="K163" s="11">
+        <f t="shared" si="8"/>
+        <v>29.14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D164" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E164" s="6">
+        <v>-135</v>
+      </c>
+      <c r="F164" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G164" s="11">
+        <v>1</v>
+      </c>
+      <c r="H164" s="11">
+        <v>1.74</v>
+      </c>
+      <c r="I164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J164" s="11">
+        <f t="shared" ref="J164:J183" si="11">IF(I164="Pending", 0,IF(I164="Win",H164-G164,-1*G164))</f>
+        <v>0.74</v>
+      </c>
+      <c r="K164" s="11">
+        <f t="shared" si="8"/>
+        <v>29.88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A165" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E165" s="6">
+        <v>215</v>
+      </c>
+      <c r="F165" s="6">
+        <v>195</v>
+      </c>
+      <c r="G165" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H165" s="11">
+        <v>1.58</v>
+      </c>
+      <c r="I165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J165" s="11">
+        <f t="shared" si="11"/>
+        <v>1.08</v>
+      </c>
+      <c r="K165" s="11">
+        <f t="shared" si="8"/>
+        <v>30.96</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E166" s="6">
+        <v>115</v>
+      </c>
+      <c r="F166" s="6">
+        <v>115</v>
+      </c>
+      <c r="G166" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H166" s="11">
+        <v>1.08</v>
+      </c>
+      <c r="I166" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J166" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K166" s="11">
+        <f t="shared" si="8"/>
+        <v>30.46</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D167" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E167" s="6">
+        <v>-104</v>
+      </c>
+      <c r="F167" s="6">
+        <v>-104</v>
+      </c>
+      <c r="G167" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H167" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="I167" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J167" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K167" s="11">
+        <f t="shared" si="8"/>
+        <v>29.96</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168" s="7">
+        <v>44918</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D168" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E168" s="6">
+        <v>-135</v>
+      </c>
+      <c r="F168" s="6">
+        <v>-135</v>
+      </c>
+      <c r="G168" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H168" s="11">
+        <v>0.87</v>
+      </c>
+      <c r="I168" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J168" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K168" s="11">
+        <f t="shared" si="8"/>
+        <v>29.46</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169" s="7">
+        <v>44920</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D169" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="E169" s="6">
+        <v>130</v>
+      </c>
+      <c r="F169" s="6">
+        <v>130</v>
+      </c>
+      <c r="G169" s="11">
+        <v>2</v>
+      </c>
+      <c r="H169" s="11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I169" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J169" s="11">
+        <f t="shared" si="11"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="K169" s="11">
+        <f t="shared" si="8"/>
+        <v>32.06</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170" s="7">
+        <v>44920</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D170" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E170" s="6">
+        <v>110</v>
+      </c>
+      <c r="F170" s="6">
+        <v>110</v>
+      </c>
+      <c r="G170" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H170" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I170" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J170" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K170" s="11">
+        <f t="shared" si="8"/>
+        <v>32.06</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171" s="7">
+        <v>44920</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E171" s="6">
+        <v>-105</v>
+      </c>
+      <c r="F171" s="6">
+        <v>-105</v>
+      </c>
+      <c r="G171" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H171" s="11">
+        <v>2.93</v>
+      </c>
+      <c r="I171" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J171" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K171" s="11">
+        <f t="shared" si="8"/>
+        <v>32.06</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172" s="7">
+        <v>44920</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E172" s="6">
+        <v>260</v>
+      </c>
+      <c r="F172" s="6">
+        <v>260</v>
+      </c>
+      <c r="G172" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H172" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="I172" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J172" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K172" s="11">
+        <f t="shared" si="8"/>
+        <v>31.560000000000002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173" s="7">
+        <v>44920</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E173" s="6">
+        <v>-115</v>
+      </c>
+      <c r="F173" s="6">
+        <v>-115</v>
+      </c>
+      <c r="G173" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H173" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="I173" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J173" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K173" s="11">
+        <f t="shared" si="8"/>
+        <v>31.060000000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174" s="7">
+        <v>44921</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E174" s="6">
+        <v>170</v>
+      </c>
+      <c r="F174" s="6">
+        <v>170</v>
+      </c>
+      <c r="G174" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H174" s="11">
+        <v>1.35</v>
+      </c>
+      <c r="I174" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J174" s="11">
+        <f t="shared" si="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K174" s="11">
+        <f t="shared" si="8"/>
+        <v>30.560000000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175" s="7">
+        <v>44921</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="E175" s="6">
+        <v>135</v>
+      </c>
+      <c r="F175" s="6">
+        <v>135</v>
+      </c>
+      <c r="G175" s="11">
+        <v>1</v>
+      </c>
+      <c r="H175" s="11">
+        <v>2.35</v>
+      </c>
+      <c r="I175" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J175" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K175" s="11">
+        <f t="shared" si="8"/>
+        <v>30.560000000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="7">
+        <v>44921</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D176" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E176" s="6">
+        <v>155</v>
+      </c>
+      <c r="F176" s="6">
+        <v>155</v>
+      </c>
+      <c r="G176" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H176" s="11">
+        <v>1.28</v>
+      </c>
+      <c r="I176" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J176" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K176" s="11">
+        <f t="shared" si="8"/>
+        <v>30.560000000000002</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177" s="7">
+        <v>44921</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D177" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E177" s="6">
+        <v>625</v>
+      </c>
+      <c r="F177" s="6">
+        <v>625</v>
+      </c>
+      <c r="G177" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H177" s="11">
+        <v>3.62</v>
+      </c>
+      <c r="I177" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J177" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K177" s="11">
+        <f t="shared" si="8"/>
+        <v>30.560000000000002</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178" s="7">
+        <v>44921</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D178" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E178" s="6">
+        <v>210</v>
+      </c>
+      <c r="F178" s="6">
+        <v>210</v>
+      </c>
+      <c r="G178" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H178" s="11">
+        <v>1.55</v>
+      </c>
+      <c r="I178" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J178" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K178" s="11">
+        <f t="shared" si="8"/>
+        <v>30.560000000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="7">
+        <v>44922</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D179" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="E179" s="6">
+        <v>120</v>
+      </c>
+      <c r="F179" s="6">
+        <v>120</v>
+      </c>
+      <c r="G179" s="11">
+        <v>1</v>
+      </c>
+      <c r="H179" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I179" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J179" s="11">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="K179" s="11">
+        <f t="shared" si="8"/>
+        <v>29.560000000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" s="7">
+        <v>44923</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E180" s="6">
+        <v>135</v>
+      </c>
+      <c r="F180" s="6">
+        <v>160</v>
+      </c>
+      <c r="G180" s="11">
+        <v>1</v>
+      </c>
+      <c r="H180" s="11">
+        <v>2.35</v>
+      </c>
+      <c r="I180" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J180" s="11">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="K180" s="11">
+        <f t="shared" si="8"/>
+        <v>28.560000000000002</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181" s="7">
+        <v>44923</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E181" s="6">
+        <v>130</v>
+      </c>
+      <c r="F181" s="6">
+        <v>120</v>
+      </c>
+      <c r="G181" s="11">
+        <v>1</v>
+      </c>
+      <c r="H181" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I181" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J181" s="11">
+        <f t="shared" si="11"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="K181" s="11">
+        <f t="shared" si="8"/>
+        <v>29.860000000000003</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182" s="7">
+        <v>44923</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="E182" s="6">
+        <v>120</v>
+      </c>
+      <c r="F182" s="6">
+        <v>120</v>
+      </c>
+      <c r="G182" s="11">
+        <v>1</v>
+      </c>
+      <c r="H182" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I182" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J182" s="11">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="K182" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E183" s="6">
+        <v>100</v>
+      </c>
+      <c r="F183" s="6">
+        <v>100</v>
+      </c>
+      <c r="G183" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H183" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="I183" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J183" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K183" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184" s="8"/>
+      <c r="B184" s="8"/>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="11"/>
+      <c r="H184" s="11"/>
+      <c r="I184" s="8"/>
+      <c r="J184" s="11"/>
+      <c r="K184" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185" s="8"/>
+      <c r="B185" s="8"/>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
+      <c r="E185" s="6"/>
+      <c r="F185" s="6"/>
+      <c r="G185" s="11"/>
+      <c r="H185" s="11"/>
+      <c r="I185" s="8"/>
+      <c r="J185" s="11"/>
+      <c r="K185" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186" s="8"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="8"/>
+      <c r="D186" s="8"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="11"/>
+      <c r="H186" s="11"/>
+      <c r="I186" s="8"/>
+      <c r="J186" s="11"/>
+      <c r="K186" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187" s="8"/>
+      <c r="B187" s="8"/>
+      <c r="C187" s="8"/>
+      <c r="D187" s="8"/>
+      <c r="E187" s="6"/>
+      <c r="F187" s="6"/>
+      <c r="G187" s="11"/>
+      <c r="H187" s="11"/>
+      <c r="I187" s="8"/>
+      <c r="J187" s="11"/>
+      <c r="K187" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" s="8"/>
+      <c r="B188" s="8"/>
+      <c r="C188" s="8"/>
+      <c r="D188" s="8"/>
+      <c r="E188" s="6"/>
+      <c r="F188" s="6"/>
+      <c r="G188" s="11"/>
+      <c r="H188" s="11"/>
+      <c r="I188" s="8"/>
+      <c r="J188" s="11"/>
+      <c r="K188" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" s="8"/>
+      <c r="B189" s="8"/>
+      <c r="C189" s="8"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="6"/>
+      <c r="F189" s="6"/>
+      <c r="G189" s="11"/>
+      <c r="H189" s="11"/>
+      <c r="I189" s="8"/>
+      <c r="J189" s="11"/>
+      <c r="K189" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" s="8"/>
+      <c r="B190" s="8"/>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="6"/>
+      <c r="F190" s="6"/>
+      <c r="G190" s="11"/>
+      <c r="H190" s="11"/>
+      <c r="I190" s="8"/>
+      <c r="J190" s="11"/>
+      <c r="K190" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" s="8"/>
+      <c r="B191" s="8"/>
+      <c r="C191" s="8"/>
+      <c r="D191" s="8"/>
+      <c r="E191" s="6"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="11"/>
+      <c r="H191" s="11"/>
+      <c r="I191" s="8"/>
+      <c r="J191" s="11"/>
+      <c r="K191" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" s="8"/>
+      <c r="B192" s="8"/>
+      <c r="C192" s="8"/>
+      <c r="D192" s="8"/>
+      <c r="E192" s="6"/>
+      <c r="F192" s="6"/>
+      <c r="G192" s="11"/>
+      <c r="H192" s="11"/>
+      <c r="I192" s="8"/>
+      <c r="J192" s="11"/>
+      <c r="K192" s="11">
+        <f t="shared" si="8"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" s="8"/>
+      <c r="B193" s="8"/>
+      <c r="C193" s="8"/>
+      <c r="D193" s="8"/>
+      <c r="E193" s="6"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="11"/>
+      <c r="H193" s="11"/>
+      <c r="I193" s="8"/>
+      <c r="J193" s="11"/>
+      <c r="K193" s="11">
+        <f t="shared" ref="K193:K194" si="12">K192+J193</f>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" s="8"/>
+      <c r="B194" s="8"/>
+      <c r="C194" s="8"/>
+      <c r="D194" s="8"/>
+      <c r="E194" s="6"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="11"/>
+      <c r="H194" s="11"/>
+      <c r="I194" s="8"/>
+      <c r="J194" s="11"/>
+      <c r="K194" s="11">
+        <f t="shared" si="12"/>
+        <v>28.860000000000003</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" s="8"/>
+      <c r="B195" s="8"/>
+      <c r="C195" s="8"/>
+      <c r="D195" s="8"/>
+      <c r="E195" s="6"/>
+      <c r="F195" s="6"/>
+      <c r="G195" s="11"/>
+      <c r="H195" s="11"/>
+      <c r="I195" s="8"/>
+      <c r="J195" s="11"/>
+      <c r="K195" s="11"/>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" s="8"/>
+      <c r="B196" s="8"/>
+      <c r="C196" s="8"/>
+      <c r="D196" s="8"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="11"/>
+      <c r="H196" s="11"/>
+      <c r="I196" s="8"/>
+      <c r="J196" s="11"/>
+      <c r="K196" s="11"/>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A197" s="8"/>
+      <c r="B197" s="8"/>
+      <c r="C197" s="8"/>
+      <c r="D197" s="8"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="11"/>
+      <c r="H197" s="11"/>
+      <c r="I197" s="8"/>
+      <c r="J197" s="11"/>
+      <c r="K197" s="11"/>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A198" s="8"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="8"/>
+      <c r="D198" s="8"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="11"/>
+      <c r="H198" s="11"/>
+      <c r="I198" s="8"/>
+      <c r="J198" s="11"/>
+      <c r="K198" s="11"/>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" s="8"/>
+      <c r="B199" s="8"/>
+      <c r="C199" s="8"/>
+      <c r="D199" s="8"/>
+      <c r="E199" s="6"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="11"/>
+      <c r="H199" s="11"/>
+      <c r="I199" s="8"/>
+      <c r="J199" s="11"/>
+      <c r="K199" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>

<commit_message>
added Draw on moneyline for soccer games
</commit_message>
<xml_diff>
--- a/betting spreadsheet.xlsx
+++ b/betting spreadsheet.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Desktop\betting-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1DDC25-CC69-4127-9EB0-26CDBABD23CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933C5192-BA6F-43E4-BEE0-96456E139066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$174</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$J$2:$J$174</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$J$2:$J$194</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="370">
   <si>
     <t>Date</t>
   </si>
@@ -1113,6 +1115,42 @@
   </si>
   <si>
     <t>Zalgiris +7.0</t>
+  </si>
+  <si>
+    <t>Leicester City vs Fulham</t>
+  </si>
+  <si>
+    <t>Fulham -0.5</t>
+  </si>
+  <si>
+    <t>Manchester City vs Everton</t>
+  </si>
+  <si>
+    <t>Draw</t>
+  </si>
+  <si>
+    <t>Minnesota vs Syracuse</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys vs Tennessee Titans</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys -11.5</t>
+  </si>
+  <si>
+    <t>Tennessee Titans</t>
+  </si>
+  <si>
+    <t>San Francisco 49ers vs Las Vegas Raiders</t>
+  </si>
+  <si>
+    <t>Point Spreads</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders +10.0</t>
+  </si>
+  <si>
+    <t>Cleveland Browns vs Washington Commanders</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1231,6 +1269,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1396,10 +1435,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$174</c:f>
+              <c:f>Sheet1!$K$2:$K$194</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="173"/>
+                <c:ptCount val="193"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -1918,6 +1957,63 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>30.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>30.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>30.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>30.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>30.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>29.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>28.560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>29.860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>28.860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>29.360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>29.360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>29.360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>30.410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>30.410000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2118,14 +2214,14 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="waterfall" uniqueId="{CAA0484D-3C77-403A-9915-3F945E5D3CB7}">
+        <cx:series layoutId="waterfall" uniqueId="{5E965C43-963E-434E-A4CB-5C48F81DED56}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:subtotals/>
@@ -3658,10 +3754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9706E5D-ABEE-4E65-AA0D-26913405A8B0}">
-  <dimension ref="A1:M199"/>
+  <dimension ref="A1:M198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I184" sqref="I184"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L193" sqref="L193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3756,8 +3852,8 @@
         <v>1.5</v>
       </c>
       <c r="M2" s="13">
-        <f>SUM(J2:J190)</f>
-        <v>28.860000000000003</v>
+        <f>SUM(J2:J194)</f>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -9750,7 +9846,7 @@
         <v>4</v>
       </c>
       <c r="J164" s="11">
-        <f t="shared" ref="J164:J183" si="11">IF(I164="Pending", 0,IF(I164="Win",H164-G164,-1*G164))</f>
+        <f t="shared" ref="J164:J190" si="11">IF(I164="Pending", 0,IF(I164="Win",H164-G164,-1*G164))</f>
         <v>0.74</v>
       </c>
       <c r="K164" s="11">
@@ -10447,130 +10543,277 @@
         <v>0.5</v>
       </c>
       <c r="H183" s="11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I183" s="8" t="s">
-        <v>251</v>
+        <v>4</v>
       </c>
       <c r="J183" s="11">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K183" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>29.360000000000003</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A184" s="8"/>
-      <c r="B184" s="8"/>
-      <c r="C184" s="8"/>
-      <c r="D184" s="8"/>
-      <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
-      <c r="G184" s="11"/>
-      <c r="H184" s="11"/>
-      <c r="I184" s="8"/>
-      <c r="J184" s="11"/>
+      <c r="A184" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="E184" s="6">
+        <v>240</v>
+      </c>
+      <c r="F184" s="6">
+        <v>240</v>
+      </c>
+      <c r="G184" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H184" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="I184" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J184" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K184" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>29.360000000000003</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A185" s="8"/>
-      <c r="B185" s="8"/>
-      <c r="C185" s="8"/>
-      <c r="D185" s="8"/>
-      <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
-      <c r="G185" s="11"/>
-      <c r="H185" s="11"/>
-      <c r="I185" s="8"/>
-      <c r="J185" s="11"/>
+      <c r="A185" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="E185" s="6">
+        <v>850</v>
+      </c>
+      <c r="F185" s="6">
+        <v>850</v>
+      </c>
+      <c r="G185" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H185" s="11">
+        <v>4.75</v>
+      </c>
+      <c r="I185" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J185" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K185" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>29.360000000000003</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A186" s="8"/>
-      <c r="B186" s="8"/>
-      <c r="C186" s="8"/>
-      <c r="D186" s="8"/>
-      <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
-      <c r="G186" s="11"/>
-      <c r="H186" s="11"/>
-      <c r="I186" s="8"/>
-      <c r="J186" s="11"/>
+      <c r="A186" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C186" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D186" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E186" s="6">
+        <v>105</v>
+      </c>
+      <c r="F186" s="6">
+        <v>105</v>
+      </c>
+      <c r="G186" s="11">
+        <v>1</v>
+      </c>
+      <c r="H186" s="11">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I186" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J186" s="11">
+        <f t="shared" si="11"/>
+        <v>1.0499999999999998</v>
+      </c>
       <c r="K186" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A187" s="8"/>
-      <c r="B187" s="8"/>
-      <c r="C187" s="8"/>
-      <c r="D187" s="8"/>
-      <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
-      <c r="G187" s="11"/>
-      <c r="H187" s="11"/>
-      <c r="I187" s="8"/>
-      <c r="J187" s="11"/>
+      <c r="A187" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D187" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="E187" s="6">
+        <v>-135</v>
+      </c>
+      <c r="F187" s="6">
+        <v>-145</v>
+      </c>
+      <c r="G187" s="11">
+        <v>1</v>
+      </c>
+      <c r="H187" s="11">
+        <v>1.74</v>
+      </c>
+      <c r="I187" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J187" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K187" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A188" s="8"/>
-      <c r="B188" s="8"/>
-      <c r="C188" s="8"/>
-      <c r="D188" s="8"/>
-      <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
-      <c r="G188" s="11"/>
-      <c r="H188" s="11"/>
-      <c r="I188" s="8"/>
-      <c r="J188" s="11"/>
+      <c r="A188" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B188" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C188" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="D188" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="E188" s="6">
+        <v>-110</v>
+      </c>
+      <c r="F188" s="6">
+        <v>-110</v>
+      </c>
+      <c r="G188" s="11">
+        <v>1</v>
+      </c>
+      <c r="H188" s="11">
+        <v>1.91</v>
+      </c>
+      <c r="I188" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J188" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K188" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A189" s="8"/>
-      <c r="B189" s="8"/>
-      <c r="C189" s="8"/>
-      <c r="D189" s="8"/>
-      <c r="E189" s="6"/>
-      <c r="F189" s="6"/>
-      <c r="G189" s="11"/>
-      <c r="H189" s="11"/>
-      <c r="I189" s="8"/>
-      <c r="J189" s="11"/>
+      <c r="A189" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B189" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="C189" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D189" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E189" s="6">
+        <v>625</v>
+      </c>
+      <c r="F189" s="6">
+        <v>625</v>
+      </c>
+      <c r="G189" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H189" s="11">
+        <v>3.62</v>
+      </c>
+      <c r="I189" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J189" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K189" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A190" s="8"/>
-      <c r="B190" s="8"/>
-      <c r="C190" s="8"/>
-      <c r="D190" s="8"/>
-      <c r="E190" s="6"/>
-      <c r="F190" s="6"/>
-      <c r="G190" s="11"/>
-      <c r="H190" s="11"/>
-      <c r="I190" s="8"/>
-      <c r="J190" s="11"/>
+      <c r="A190" s="7">
+        <v>44924</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D190" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E190" s="6">
+        <v>-150</v>
+      </c>
+      <c r="F190" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G190" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H190" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="I190" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J190" s="11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
       <c r="K190" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
@@ -10586,7 +10829,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
@@ -10602,7 +10845,7 @@
       <c r="J192" s="11"/>
       <c r="K192" s="11">
         <f t="shared" si="8"/>
-        <v>28.860000000000003</v>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
@@ -10617,8 +10860,8 @@
       <c r="I193" s="8"/>
       <c r="J193" s="11"/>
       <c r="K193" s="11">
-        <f t="shared" ref="K193:K194" si="12">K192+J193</f>
-        <v>28.860000000000003</v>
+        <f t="shared" ref="K193" si="12">K192+J193</f>
+        <v>30.410000000000004</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
@@ -10632,10 +10875,7 @@
       <c r="H194" s="11"/>
       <c r="I194" s="8"/>
       <c r="J194" s="11"/>
-      <c r="K194" s="11">
-        <f t="shared" si="12"/>
-        <v>28.860000000000003</v>
-      </c>
+      <c r="K194" s="11"/>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="8"/>
@@ -10688,19 +10928,6 @@
       <c r="I198" s="8"/>
       <c r="J198" s="11"/>
       <c r="K198" s="11"/>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A199" s="8"/>
-      <c r="B199" s="8"/>
-      <c r="C199" s="8"/>
-      <c r="D199" s="8"/>
-      <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
-      <c r="G199" s="11"/>
-      <c r="H199" s="11"/>
-      <c r="I199" s="8"/>
-      <c r="J199" s="11"/>
-      <c r="K199" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>

<commit_message>
different LOL leagues, australian open, and la liga
</commit_message>
<xml_diff>
--- a/betting spreadsheet.xlsx
+++ b/betting spreadsheet.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacks\Desktop\betting-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9C0B14-1CD4-4B5C-95A1-3C927D763ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB73B758-1BB9-4731-87F4-025D55EF42B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="586" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
+    <workbookView xWindow="6000" yWindow="1110" windowWidth="20265" windowHeight="11805" tabRatio="586" xr2:uid="{B8F52F6D-E50B-46F2-88DA-98A7B049B083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$225</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$J$2:$J$283</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="534">
   <si>
     <t>Date</t>
   </si>
@@ -1325,7 +1325,322 @@
     <t>Under 193.0</t>
   </si>
   <si>
-    <t>Carolina Hurricanes vs Columbus Blue Jackets</t>
+    <t>DRX -1.5</t>
+  </si>
+  <si>
+    <t>DAMWON vs DRX</t>
+  </si>
+  <si>
+    <t>Arsenal vs Manchester United</t>
+  </si>
+  <si>
+    <t>Arsenal -1.0 -1.5</t>
+  </si>
+  <si>
+    <t>St. John's vs Providence</t>
+  </si>
+  <si>
+    <t>Creighton vs Connecticut</t>
+  </si>
+  <si>
+    <t>Creighton +6.0</t>
+  </si>
+  <si>
+    <t>Providence -9.0</t>
+  </si>
+  <si>
+    <t>Wichita State vs South Florida</t>
+  </si>
+  <si>
+    <t>Over 126.5</t>
+  </si>
+  <si>
+    <t>Zhejiang Golden Bulls vs Jilin Northeast Tigers</t>
+  </si>
+  <si>
+    <t>Nicolas Jarry vs Otto Virtanen</t>
+  </si>
+  <si>
+    <t>Otto Virtanen</t>
+  </si>
+  <si>
+    <t>Sonay Kartal vs Elizabeth Mandlik</t>
+  </si>
+  <si>
+    <t>Over 22.5</t>
+  </si>
+  <si>
+    <t>Seattle Kraken vs Montreal Canadiens</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks vs San Francisco 49ers</t>
+  </si>
+  <si>
+    <t>Seattle Seahwaks</t>
+  </si>
+  <si>
+    <t>Colgate vs Army</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Alex Bolt vs Matteo Arnaldi</t>
+  </si>
+  <si>
+    <t>Matteo Arnaldi -4.0</t>
+  </si>
+  <si>
+    <t>Jurij Rodionov vs Adrian Andreev</t>
+  </si>
+  <si>
+    <t>Under 22.0</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys vs Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers +3.5</t>
+  </si>
+  <si>
+    <t>Butler vs St. John's</t>
+  </si>
+  <si>
+    <t>Butler</t>
+  </si>
+  <si>
+    <t>Toledo vs Kent State</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Marco Trungelliti vs Marc Polmans</t>
+  </si>
+  <si>
+    <t>Marco Trungelliti</t>
+  </si>
+  <si>
+    <t>Central Michigan vs Northern Illinois</t>
+  </si>
+  <si>
+    <t>Northern Illinois</t>
+  </si>
+  <si>
+    <t>Alexandre Muller vs Yu Hsiou Hsu</t>
+  </si>
+  <si>
+    <t>Pavel Kotov vs Ernesto Escobedo</t>
+  </si>
+  <si>
+    <t>Ernesto Escobedo +4.0</t>
+  </si>
+  <si>
+    <t>Dominic Stephan Stricker vs Enzo Couacaud</t>
+  </si>
+  <si>
+    <t>Enzo Couacaud</t>
+  </si>
+  <si>
+    <t>Furman vs Mercer</t>
+  </si>
+  <si>
+    <t>Mercer</t>
+  </si>
+  <si>
+    <t>Jan-Lennard Struff vs Tristan Schoolkate</t>
+  </si>
+  <si>
+    <t>Jan-Lennard Struff -4.0</t>
+  </si>
+  <si>
+    <t>Towson vs Delaware</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Leolia Jeanjean vs Lesia Tsurenko</t>
+  </si>
+  <si>
+    <t>Lesia Tsurenko -5.0</t>
+  </si>
+  <si>
+    <t>Juan Pablo Varillas vs Yosuke Watanuki</t>
+  </si>
+  <si>
+    <t>Juan Pablo Varillas +4.5</t>
+  </si>
+  <si>
+    <t>Stefanos Tsitsipas vs Quentin Halys</t>
+  </si>
+  <si>
+    <t>Quentin Halys +6.5</t>
+  </si>
+  <si>
+    <t>Marcos Giron vs Daniil Medvedev</t>
+  </si>
+  <si>
+    <t>Marcos Giron +9.0</t>
+  </si>
+  <si>
+    <t>Max Purcell vs Emil Ruusuvuori</t>
+  </si>
+  <si>
+    <t>Emil Ruusuvuori -6.0</t>
+  </si>
+  <si>
+    <t>Emma Raducanu vs Tamara Korpatsch</t>
+  </si>
+  <si>
+    <t>Under 18.0</t>
+  </si>
+  <si>
+    <t>Marta Kostyuk vs Amanda Anisimova</t>
+  </si>
+  <si>
+    <t>Under 20.5</t>
+  </si>
+  <si>
+    <t>Miami Dolphins vs Buffalo Bills</t>
+  </si>
+  <si>
+    <t>Miami Dolphins</t>
+  </si>
+  <si>
+    <t>Francisco Cerundolo vs Guido Pella</t>
+  </si>
+  <si>
+    <t>Francisco Cerundolo -8.0</t>
+  </si>
+  <si>
+    <t>Seattle Kraken vs Chicago Blackhawks</t>
+  </si>
+  <si>
+    <t>Seattle Kraken -2.5</t>
+  </si>
+  <si>
+    <t>Montreal Canadiens vs New York Islanders</t>
+  </si>
+  <si>
+    <t>New York Islanders -2.5</t>
+  </si>
+  <si>
+    <t>Kentucky vs Tennessee</t>
+  </si>
+  <si>
+    <t>Kentucky +9.0</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars vs Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>Diane Parry vs Taylor Townsend</t>
+  </si>
+  <si>
+    <t>Diane Parry +2.5</t>
+  </si>
+  <si>
+    <t>Weibo Gaming vs Top Esports</t>
+  </si>
+  <si>
+    <t>Weibo Gaming -1.5</t>
+  </si>
+  <si>
+    <t>Petra Martic vs Viktorija Golubic</t>
+  </si>
+  <si>
+    <t>Petra Martic -3.0</t>
+  </si>
+  <si>
+    <t>Thanasi Kokkinakis vs Fabio Fognini</t>
+  </si>
+  <si>
+    <t>Thanasi Kokkinakis -6.5</t>
+  </si>
+  <si>
+    <t>Daria Kasatkina vs Varvara Gracheva</t>
+  </si>
+  <si>
+    <t>Daria Kasatkina -7.0</t>
+  </si>
+  <si>
+    <t>Tennessee vs Mississippi State</t>
+  </si>
+  <si>
+    <t>Columbus Blue Jackets vs Nashville Predators</t>
+  </si>
+  <si>
+    <t>Mississippi State</t>
+  </si>
+  <si>
+    <t>Shuai Zhang vs Patricia Maria Tig</t>
+  </si>
+  <si>
+    <t>Buffalo Sabres vs Chicago Blackhawks</t>
+  </si>
+  <si>
+    <t>Over 7.5</t>
+  </si>
+  <si>
+    <t>T1 vs Gen.G</t>
+  </si>
+  <si>
+    <t>Gen.G</t>
+  </si>
+  <si>
+    <t>Hubert Hurkacz vs Lorenzo Sonego</t>
+  </si>
+  <si>
+    <t>Lorenzo Sonego +4.0</t>
+  </si>
+  <si>
+    <t>Taylor Fritz vs Alexei Popyrin</t>
+  </si>
+  <si>
+    <t>Alexei Popyrin +7.0</t>
+  </si>
+  <si>
+    <t>Alejandro Davidovich Fokina vs Tommy Paul</t>
+  </si>
+  <si>
+    <t>Alejandro Davidovich Fokina +5.0</t>
+  </si>
+  <si>
+    <t>Michael Mmoh vs Alexander Zverev</t>
+  </si>
+  <si>
+    <t>Michael Mmoh +5.0</t>
+  </si>
+  <si>
+    <t>Rare Atom vs Ninjas in Pyjamas</t>
+  </si>
+  <si>
+    <t>Rare Atoms</t>
+  </si>
+  <si>
+    <t>Enzo Couacaud vs Novak Djokovic</t>
+  </si>
+  <si>
+    <t>Novak Djokovic -9.5</t>
+  </si>
+  <si>
+    <t>Lgd Gaming vs OMG</t>
+  </si>
+  <si>
+    <t>Lgd Gaming</t>
+  </si>
+  <si>
+    <t>Under 20.0</t>
+  </si>
+  <si>
+    <t>Golden State Warriors vs Boston Celtics</t>
+  </si>
+  <si>
+    <t>Linda Fruhvirtova vs Marketa Vondrousova</t>
+  </si>
+  <si>
+    <t>Shuai Zhang vs Katie Volynets</t>
   </si>
 </sst>
 </file>
@@ -1613,10 +1928,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$225</c:f>
+              <c:f>Sheet1!$K$2:$K$283</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="224"/>
+                <c:ptCount val="282"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -2221,73 +2536,247 @@
                   <c:v>49.03</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>49.03</c:v>
+                  <c:v>47.03</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>48.53</c:v>
+                  <c:v>46.53</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>48.03</c:v>
+                  <c:v>46.03</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>47.03</c:v>
+                  <c:v>45.03</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>46.53</c:v>
+                  <c:v>44.53</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>46.03</c:v>
+                  <c:v>44.03</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>46.03</c:v>
+                  <c:v>42.03</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>45.03</c:v>
+                  <c:v>41.03</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>46.03</c:v>
+                  <c:v>42.03</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>46.03</c:v>
+                  <c:v>39.53</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>46.03</c:v>
+                  <c:v>40.53</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>45.53</c:v>
+                  <c:v>40.03</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>47.25</c:v>
+                  <c:v>41.75</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>52.85</c:v>
+                  <c:v>47.35</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>52.85</c:v>
+                  <c:v>47.35</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>59.6</c:v>
+                  <c:v>54.1</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>59.6</c:v>
+                  <c:v>53.1</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>60.75</c:v>
+                  <c:v>54.25</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>60.75</c:v>
+                  <c:v>53.75</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>60.75</c:v>
+                  <c:v>52.25</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>61.7</c:v>
+                  <c:v>53.2</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>61.7</c:v>
+                  <c:v>52.7</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>61.7</c:v>
+                  <c:v>52.7</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>51.7</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>50.2</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>54.11</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>53.61</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>51.61</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>52.81</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>53.53</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>53.03</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>52.53</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>51.03</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>52.75</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>51.75</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>50.25</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>48.75</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>51.95</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>52.95</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>51.45</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>53.650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>56.850000000000009</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>56.350000000000009</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>58.750000000000007</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>60.930000000000007</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>62.180000000000007</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>65.48</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>63.480000000000004</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>65.19</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>60.19</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>58.69</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>64.64</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>68.69</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>67.19</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>60.69</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>64.789999999999992</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>62.789999999999992</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>64.809999999999988</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>64.809999999999988</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>61.809999999999988</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>59.809999999999988</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>66.309999999999988</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>69.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>66.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>64.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>69.11</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>64.61</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>62.61</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>60.61</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>69.010000000000005</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>72.25</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>75.709999999999994</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>79.61</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>79.61</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>81.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2495,7 +2984,7 @@
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="waterfall" uniqueId="{FF5F689A-0C12-4E6B-BCB8-F028EF2E203C}">
+        <cx:series layoutId="waterfall" uniqueId="{5118BAE7-A0E5-4016-9FAA-B48997407949}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:subtotals/>
@@ -4039,7 +4528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4047,10 +4536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9706E5D-ABEE-4E65-AA0D-26913405A8B0}">
-  <dimension ref="A1:M412"/>
+  <dimension ref="A1:M404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M219" sqref="M219"/>
+    <sheetView tabSelected="1" topLeftCell="A267" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F280" sqref="F280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4145,8 +4634,8 @@
         <v>1.5</v>
       </c>
       <c r="M2" s="13">
-        <f>SUM(J2:J225)</f>
-        <v>61.7</v>
+        <f>SUM(J2:J283)</f>
+        <v>81.99</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -11216,7 +11705,7 @@
         <v>0.66999999999999993</v>
       </c>
       <c r="K193" s="11">
-        <f t="shared" ref="K193:K236" si="14">K192+J193</f>
+        <f t="shared" ref="K193:K257" si="14">K192+J193</f>
         <v>45.220000000000006</v>
       </c>
     </row>
@@ -11570,7 +12059,7 @@
         <v>265</v>
       </c>
       <c r="F203" s="6">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="G203" s="11">
         <v>2</v>
@@ -11579,15 +12068,15 @@
         <v>5.3</v>
       </c>
       <c r="I203" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J203" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K203" s="11">
         <f t="shared" si="14"/>
-        <v>49.03</v>
+        <v>47.03</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
@@ -11624,7 +12113,7 @@
       </c>
       <c r="K204" s="11">
         <f t="shared" si="14"/>
-        <v>48.53</v>
+        <v>46.53</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
@@ -11661,7 +12150,7 @@
       </c>
       <c r="K205" s="11">
         <f t="shared" si="14"/>
-        <v>48.03</v>
+        <v>46.03</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
@@ -11698,7 +12187,7 @@
       </c>
       <c r="K206" s="11">
         <f t="shared" si="14"/>
-        <v>47.03</v>
+        <v>45.03</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
@@ -11735,7 +12224,7 @@
       </c>
       <c r="K207" s="11">
         <f t="shared" si="14"/>
-        <v>46.53</v>
+        <v>44.53</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
@@ -11772,7 +12261,7 @@
       </c>
       <c r="K208" s="11">
         <f t="shared" si="14"/>
-        <v>46.03</v>
+        <v>44.03</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
@@ -11792,7 +12281,7 @@
         <v>115</v>
       </c>
       <c r="F209" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G209" s="11">
         <v>2</v>
@@ -11801,15 +12290,15 @@
         <v>4.3</v>
       </c>
       <c r="I209" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J209" s="11">
         <f t="shared" ref="J209:J211" si="16">IF(I209="Pending", 0,IF(I209="Win",H209-G209,-1*G209))</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K209" s="11">
         <f t="shared" si="14"/>
-        <v>46.03</v>
+        <v>42.03</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
@@ -11846,7 +12335,7 @@
       </c>
       <c r="K210" s="11">
         <f t="shared" si="14"/>
-        <v>45.03</v>
+        <v>41.03</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
@@ -11883,7 +12372,7 @@
       </c>
       <c r="K211" s="11">
         <f t="shared" si="14"/>
-        <v>46.03</v>
+        <v>42.03</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
@@ -11903,24 +12392,24 @@
         <v>135</v>
       </c>
       <c r="F212" s="6">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="G212" s="11">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="H212" s="11">
-        <v>3.52</v>
+        <v>5.88</v>
       </c>
       <c r="I212" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J212" s="11">
-        <f t="shared" ref="J212:J224" si="17">IF(I212="Pending", 0,IF(I212="Win",H212-G212,-1*G212))</f>
-        <v>0</v>
+        <f t="shared" ref="J212:J280" si="17">IF(I212="Pending", 0,IF(I212="Win",H212-G212,-1*G212))</f>
+        <v>-2.5</v>
       </c>
       <c r="K212" s="11">
         <f t="shared" ref="K212" si="18">K211+J212</f>
-        <v>46.03</v>
+        <v>39.53</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
@@ -11949,15 +12438,15 @@
         <v>2.5</v>
       </c>
       <c r="I213" s="8" t="s">
-        <v>251</v>
+        <v>4</v>
       </c>
       <c r="J213" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K213" s="11">
         <f t="shared" si="14"/>
-        <v>46.03</v>
+        <v>40.53</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
@@ -11994,7 +12483,7 @@
       </c>
       <c r="K214" s="11">
         <f t="shared" si="14"/>
-        <v>45.53</v>
+        <v>40.03</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
@@ -12031,7 +12520,7 @@
       </c>
       <c r="K215" s="11">
         <f t="shared" si="14"/>
-        <v>47.25</v>
+        <v>41.75</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
@@ -12068,7 +12557,7 @@
       </c>
       <c r="K216" s="11">
         <f t="shared" si="14"/>
-        <v>52.85</v>
+        <v>47.35</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
@@ -12088,7 +12577,7 @@
         <v>-108</v>
       </c>
       <c r="F217" s="6">
-        <v>-112</v>
+        <v>-115</v>
       </c>
       <c r="G217" s="11">
         <v>1</v>
@@ -12105,7 +12594,7 @@
       </c>
       <c r="K217" s="11">
         <f t="shared" si="14"/>
-        <v>52.85</v>
+        <v>47.35</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
@@ -12142,7 +12631,7 @@
       </c>
       <c r="K218" s="11">
         <f t="shared" si="14"/>
-        <v>59.6</v>
+        <v>54.1</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
@@ -12171,15 +12660,15 @@
         <v>3.25</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J219" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K219" s="11">
         <f t="shared" si="14"/>
-        <v>59.6</v>
+        <v>53.1</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
@@ -12216,7 +12705,7 @@
       </c>
       <c r="K220" s="11">
         <f t="shared" si="14"/>
-        <v>60.75</v>
+        <v>54.25</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
@@ -12236,7 +12725,7 @@
         <v>625</v>
       </c>
       <c r="F221" s="6">
-        <v>625</v>
+        <v>700</v>
       </c>
       <c r="G221" s="11">
         <v>0.5</v>
@@ -12245,15 +12734,15 @@
         <v>3.62</v>
       </c>
       <c r="I221" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J221" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K221" s="11">
         <f t="shared" si="14"/>
-        <v>60.75</v>
+        <v>53.75</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
@@ -12282,15 +12771,15 @@
         <v>4.95</v>
       </c>
       <c r="I222" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J222" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="K222" s="11">
         <f t="shared" si="14"/>
-        <v>60.75</v>
+        <v>52.25</v>
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
@@ -12327,822 +12816,2154 @@
       </c>
       <c r="K223" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="7">
-        <v>44932</v>
+        <v>44933</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C224" s="8" t="s">
         <v>214</v>
       </c>
       <c r="D224" s="8" t="s">
-        <v>29</v>
+        <v>428</v>
       </c>
       <c r="E224" s="6">
-        <v>135</v>
+        <v>550</v>
       </c>
       <c r="F224" s="6">
-        <v>135</v>
+        <v>750</v>
       </c>
       <c r="G224" s="11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H224" s="11">
-        <v>2.35</v>
+        <v>3.25</v>
       </c>
       <c r="I224" s="8" t="s">
-        <v>251</v>
+        <v>5</v>
       </c>
       <c r="J224" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K224" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A225" s="8"/>
-      <c r="B225" s="8"/>
-      <c r="C225" s="8"/>
-      <c r="D225" s="8"/>
-      <c r="E225" s="6"/>
-      <c r="F225" s="6"/>
-      <c r="G225" s="11"/>
-      <c r="H225" s="11"/>
-      <c r="I225" s="8"/>
-      <c r="J225" s="11"/>
+      <c r="A225" s="7">
+        <v>44933</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C225" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D225" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="E225" s="6">
+        <v>220</v>
+      </c>
+      <c r="F225" s="6">
+        <v>210</v>
+      </c>
+      <c r="G225" s="11">
+        <v>1</v>
+      </c>
+      <c r="H225" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="I225" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J225" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="K225" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A226" s="8"/>
-      <c r="B226" s="8"/>
-      <c r="C226" s="8"/>
-      <c r="D226" s="8"/>
-      <c r="E226" s="6"/>
-      <c r="F226" s="6"/>
-      <c r="G226" s="11"/>
-      <c r="H226" s="11"/>
-      <c r="I226" s="8"/>
-      <c r="J226" s="11"/>
+      <c r="A226" s="7">
+        <v>44933</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C226" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D226" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E226" s="6">
+        <v>115</v>
+      </c>
+      <c r="F226" s="6">
+        <v>-105</v>
+      </c>
+      <c r="G226" s="11">
+        <v>1</v>
+      </c>
+      <c r="H226" s="11">
+        <v>2.15</v>
+      </c>
+      <c r="I226" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J226" s="11">
+        <f t="shared" si="17"/>
+        <v>-1</v>
+      </c>
       <c r="K226" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>51.7</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A227" s="8"/>
-      <c r="B227" s="8"/>
-      <c r="C227" s="8"/>
-      <c r="D227" s="8"/>
-      <c r="E227" s="6"/>
-      <c r="F227" s="6"/>
-      <c r="G227" s="11"/>
-      <c r="H227" s="11"/>
-      <c r="I227" s="8"/>
-      <c r="J227" s="11"/>
+      <c r="A227" s="7">
+        <v>44933</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C227" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D227" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="E227" s="6">
+        <v>145</v>
+      </c>
+      <c r="F227" s="6">
+        <v>145</v>
+      </c>
+      <c r="G227" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H227" s="11">
+        <v>3.68</v>
+      </c>
+      <c r="I227" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J227" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
       <c r="K227" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>50.2</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A228" s="8"/>
-      <c r="B228" s="8"/>
-      <c r="C228" s="8"/>
-      <c r="D228" s="8"/>
-      <c r="E228" s="6"/>
-      <c r="F228" s="6"/>
-      <c r="G228" s="11"/>
-      <c r="H228" s="11"/>
-      <c r="I228" s="8"/>
-      <c r="J228" s="11"/>
+      <c r="A228" s="7">
+        <v>44934</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="C228" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D228" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E228" s="6">
+        <v>-115</v>
+      </c>
+      <c r="F228" s="6">
+        <v>-115</v>
+      </c>
+      <c r="G228" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="H228" s="11">
+        <v>8.41</v>
+      </c>
+      <c r="I228" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J228" s="11">
+        <f t="shared" si="17"/>
+        <v>3.91</v>
+      </c>
       <c r="K228" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>54.11</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A229" s="8"/>
-      <c r="B229" s="8"/>
-      <c r="C229" s="8"/>
-      <c r="D229" s="8"/>
-      <c r="E229" s="6"/>
-      <c r="F229" s="6"/>
-      <c r="G229" s="11"/>
-      <c r="H229" s="11"/>
-      <c r="I229" s="8"/>
-      <c r="J229" s="11"/>
+      <c r="A229" s="7">
+        <v>44934</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C229" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D229" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E229" s="6">
+        <v>1100</v>
+      </c>
+      <c r="F229" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G229" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H229" s="11">
+        <v>6</v>
+      </c>
+      <c r="I229" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J229" s="11">
+        <f t="shared" si="17"/>
+        <v>-0.5</v>
+      </c>
       <c r="K229" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>53.61</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A230" s="8"/>
-      <c r="B230" s="8"/>
-      <c r="C230" s="8"/>
-      <c r="D230" s="8"/>
-      <c r="E230" s="6"/>
-      <c r="F230" s="6"/>
-      <c r="G230" s="11"/>
-      <c r="H230" s="11"/>
-      <c r="I230" s="8"/>
-      <c r="J230" s="11"/>
+      <c r="A230" s="7">
+        <v>44934</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="C230" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D230" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E230" s="6">
+        <v>140</v>
+      </c>
+      <c r="F230" s="6">
+        <v>140</v>
+      </c>
+      <c r="G230" s="11">
+        <v>2</v>
+      </c>
+      <c r="H230" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="I230" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J230" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
       <c r="K230" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>51.61</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A231" s="8"/>
-      <c r="B231" s="8"/>
-      <c r="C231" s="8"/>
-      <c r="D231" s="8"/>
-      <c r="E231" s="6"/>
-      <c r="F231" s="6"/>
-      <c r="G231" s="11"/>
-      <c r="H231" s="11"/>
-      <c r="I231" s="8"/>
-      <c r="J231" s="11"/>
+      <c r="A231" s="7">
+        <v>44934</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="C231" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D231" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="E231" s="6">
+        <v>120</v>
+      </c>
+      <c r="F231" s="6">
+        <v>120</v>
+      </c>
+      <c r="G231" s="11">
+        <v>1</v>
+      </c>
+      <c r="H231" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I231" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J231" s="11">
+        <f t="shared" si="17"/>
+        <v>1.2000000000000002</v>
+      </c>
       <c r="K231" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>52.81</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A232" s="8"/>
-      <c r="B232" s="8"/>
-      <c r="C232" s="8"/>
-      <c r="D232" s="8"/>
-      <c r="E232" s="6"/>
-      <c r="F232" s="6"/>
-      <c r="G232" s="11"/>
-      <c r="H232" s="11"/>
-      <c r="I232" s="8"/>
-      <c r="J232" s="11"/>
+      <c r="A232" s="7">
+        <v>44935</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="C232" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D232" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E232" s="6">
+        <v>145</v>
+      </c>
+      <c r="F232" s="6">
+        <v>145</v>
+      </c>
+      <c r="G232" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H232" s="11">
+        <v>1.22</v>
+      </c>
+      <c r="I232" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J232" s="11">
+        <f t="shared" si="17"/>
+        <v>0.72</v>
+      </c>
       <c r="K232" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>53.53</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A233" s="8"/>
-      <c r="B233" s="8"/>
-      <c r="C233" s="8"/>
-      <c r="D233" s="8"/>
-      <c r="E233" s="6"/>
-      <c r="F233" s="6"/>
-      <c r="G233" s="11"/>
-      <c r="H233" s="11"/>
-      <c r="I233" s="8"/>
-      <c r="J233" s="11"/>
+      <c r="A233" s="7">
+        <v>44935</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="C233" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D233" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="E233" s="6">
+        <v>390</v>
+      </c>
+      <c r="F233" s="6">
+        <v>425</v>
+      </c>
+      <c r="G233" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H233" s="11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I233" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J233" s="11">
+        <f t="shared" si="17"/>
+        <v>-0.5</v>
+      </c>
       <c r="K233" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>53.03</v>
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A234" s="8"/>
-      <c r="B234" s="8"/>
-      <c r="C234" s="8"/>
-      <c r="D234" s="8"/>
-      <c r="E234" s="6"/>
-      <c r="F234" s="6"/>
-      <c r="G234" s="11"/>
-      <c r="H234" s="11"/>
-      <c r="I234" s="8"/>
-      <c r="J234" s="11"/>
+      <c r="A234" s="7">
+        <v>44935</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D234" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="E234" s="6">
+        <v>280</v>
+      </c>
+      <c r="F234" s="6">
+        <v>275</v>
+      </c>
+      <c r="G234" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H234" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="I234" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J234" s="11">
+        <f t="shared" si="17"/>
+        <v>-0.5</v>
+      </c>
       <c r="K234" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>52.53</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A235" s="8"/>
-      <c r="B235" s="8"/>
-      <c r="C235" s="8"/>
-      <c r="D235" s="8"/>
-      <c r="E235" s="6"/>
-      <c r="F235" s="6"/>
-      <c r="G235" s="11"/>
-      <c r="H235" s="11"/>
-      <c r="I235" s="8"/>
-      <c r="J235" s="11"/>
+      <c r="A235" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="C235" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D235" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="E235" s="6">
+        <v>135</v>
+      </c>
+      <c r="F235" s="6">
+        <v>135</v>
+      </c>
+      <c r="G235" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H235" s="11">
+        <v>3.52</v>
+      </c>
+      <c r="I235" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J235" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
       <c r="K235" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>51.03</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A236" s="8"/>
-      <c r="B236" s="8"/>
-      <c r="C236" s="8"/>
-      <c r="D236" s="8"/>
-      <c r="E236" s="6"/>
-      <c r="F236" s="6"/>
-      <c r="G236" s="11"/>
-      <c r="H236" s="11"/>
-      <c r="I236" s="8"/>
-      <c r="J236" s="11"/>
+      <c r="A236" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C236" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D236" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="E236" s="6">
+        <v>115</v>
+      </c>
+      <c r="F236" s="6">
+        <v>115</v>
+      </c>
+      <c r="G236" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H236" s="11">
+        <v>3.22</v>
+      </c>
+      <c r="I236" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J236" s="11">
+        <f t="shared" si="17"/>
+        <v>1.7200000000000002</v>
+      </c>
       <c r="K236" s="11">
         <f t="shared" si="14"/>
-        <v>61.7</v>
+        <v>52.75</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" s="8"/>
-      <c r="B237" s="8"/>
-      <c r="C237" s="8"/>
-      <c r="D237" s="8"/>
-      <c r="E237" s="6"/>
-      <c r="F237" s="6"/>
-      <c r="G237" s="11"/>
-      <c r="H237" s="11"/>
-      <c r="I237" s="8"/>
-      <c r="J237" s="11"/>
-      <c r="K237" s="11"/>
+      <c r="A237" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D237" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="E237" s="6">
+        <v>-130</v>
+      </c>
+      <c r="F237" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G237" s="11">
+        <v>1</v>
+      </c>
+      <c r="H237" s="11">
+        <v>1.77</v>
+      </c>
+      <c r="I237" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J237" s="11">
+        <f t="shared" si="17"/>
+        <v>-1</v>
+      </c>
+      <c r="K237" s="11">
+        <f t="shared" si="14"/>
+        <v>51.75</v>
+      </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A238" s="8"/>
-      <c r="B238" s="8"/>
-      <c r="C238" s="8"/>
-      <c r="D238" s="8"/>
-      <c r="E238" s="6"/>
-      <c r="F238" s="6"/>
-      <c r="G238" s="11"/>
-      <c r="H238" s="11"/>
-      <c r="I238" s="8"/>
-      <c r="J238" s="11"/>
-      <c r="K238" s="11"/>
+      <c r="A238" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C238" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D238" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="E238" s="6">
+        <v>150</v>
+      </c>
+      <c r="F238" s="6">
+        <v>145</v>
+      </c>
+      <c r="G238" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H238" s="11">
+        <v>3.75</v>
+      </c>
+      <c r="I238" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J238" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K238" s="11">
+        <f t="shared" si="14"/>
+        <v>50.25</v>
+      </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A239" s="8"/>
-      <c r="B239" s="8"/>
-      <c r="C239" s="8"/>
-      <c r="D239" s="8"/>
-      <c r="E239" s="6"/>
-      <c r="F239" s="6"/>
-      <c r="G239" s="11"/>
-      <c r="H239" s="11"/>
-      <c r="I239" s="8"/>
-      <c r="J239" s="11"/>
-      <c r="K239" s="11"/>
+      <c r="A239" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D239" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="E239" s="6">
+        <v>145</v>
+      </c>
+      <c r="F239" s="6">
+        <v>150</v>
+      </c>
+      <c r="G239" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H239" s="11">
+        <v>3.68</v>
+      </c>
+      <c r="I239" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J239" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K239" s="11">
+        <f t="shared" si="14"/>
+        <v>48.75</v>
+      </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A240" s="8"/>
-      <c r="B240" s="8"/>
-      <c r="C240" s="8"/>
-      <c r="D240" s="8"/>
-      <c r="E240" s="6"/>
-      <c r="F240" s="6"/>
-      <c r="G240" s="11"/>
-      <c r="H240" s="11"/>
-      <c r="I240" s="8"/>
-      <c r="J240" s="11"/>
-      <c r="K240" s="11"/>
+      <c r="A240" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C240" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D240" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="E240" s="6">
+        <v>160</v>
+      </c>
+      <c r="F240" s="6">
+        <v>160</v>
+      </c>
+      <c r="G240" s="11">
+        <v>2</v>
+      </c>
+      <c r="H240" s="11">
+        <v>5.2</v>
+      </c>
+      <c r="I240" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J240" s="11">
+        <f t="shared" si="17"/>
+        <v>3.2</v>
+      </c>
+      <c r="K240" s="11">
+        <f t="shared" si="14"/>
+        <v>51.95</v>
+      </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A241" s="8"/>
-      <c r="B241" s="8"/>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="11"/>
-      <c r="H241" s="11"/>
-      <c r="I241" s="8"/>
-      <c r="J241" s="11"/>
-      <c r="K241" s="11"/>
+      <c r="A241" s="7">
+        <v>44936</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C241" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D241" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="E241" s="6">
+        <v>100</v>
+      </c>
+      <c r="F241" s="6">
+        <v>-110</v>
+      </c>
+      <c r="G241" s="11">
+        <v>1</v>
+      </c>
+      <c r="H241" s="11">
+        <v>2</v>
+      </c>
+      <c r="I241" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J241" s="11">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K241" s="11">
+        <f>K240+J241</f>
+        <v>52.95</v>
+      </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A242" s="8"/>
-      <c r="B242" s="8"/>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="6"/>
-      <c r="F242" s="6"/>
-      <c r="G242" s="11"/>
-      <c r="H242" s="11"/>
-      <c r="I242" s="8"/>
-      <c r="J242" s="11"/>
-      <c r="K242" s="11"/>
+      <c r="A242" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="C242" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D242" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="E242" s="6">
+        <v>110</v>
+      </c>
+      <c r="F242" s="6">
+        <v>110</v>
+      </c>
+      <c r="G242" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H242" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="I242" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J242" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K242" s="11">
+        <f t="shared" si="14"/>
+        <v>51.45</v>
+      </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A243" s="8"/>
-      <c r="B243" s="8"/>
-      <c r="C243" s="8"/>
-      <c r="D243" s="8"/>
-      <c r="E243" s="6"/>
-      <c r="F243" s="6"/>
-      <c r="G243" s="11"/>
-      <c r="H243" s="11"/>
-      <c r="I243" s="8"/>
-      <c r="J243" s="11"/>
-      <c r="K243" s="11"/>
+      <c r="A243" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="C243" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D243" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="E243" s="6">
+        <v>110</v>
+      </c>
+      <c r="F243" s="6">
+        <v>-155</v>
+      </c>
+      <c r="G243" s="11">
+        <v>2</v>
+      </c>
+      <c r="H243" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="I243" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J243" s="11">
+        <f t="shared" si="17"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K243" s="11">
+        <f t="shared" si="14"/>
+        <v>53.650000000000006</v>
+      </c>
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A244" s="8"/>
-      <c r="B244" s="8"/>
-      <c r="C244" s="8"/>
-      <c r="D244" s="8"/>
-      <c r="E244" s="6"/>
-      <c r="F244" s="6"/>
-      <c r="G244" s="11"/>
-      <c r="H244" s="11"/>
-      <c r="I244" s="8"/>
-      <c r="J244" s="11"/>
-      <c r="K244" s="11"/>
+      <c r="A244" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="C244" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D244" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="E244" s="6">
+        <v>160</v>
+      </c>
+      <c r="F244" s="6">
+        <v>150</v>
+      </c>
+      <c r="G244" s="11">
+        <v>2</v>
+      </c>
+      <c r="H244" s="11">
+        <v>5.2</v>
+      </c>
+      <c r="I244" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J244" s="11">
+        <f t="shared" si="17"/>
+        <v>3.2</v>
+      </c>
+      <c r="K244" s="11">
+        <f t="shared" si="14"/>
+        <v>56.850000000000009</v>
+      </c>
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A245" s="8"/>
-      <c r="B245" s="8"/>
-      <c r="C245" s="8"/>
-      <c r="D245" s="8"/>
-      <c r="E245" s="6"/>
-      <c r="F245" s="6"/>
-      <c r="G245" s="11"/>
-      <c r="H245" s="11"/>
-      <c r="I245" s="8"/>
-      <c r="J245" s="11"/>
-      <c r="K245" s="11"/>
+      <c r="A245" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C245" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D245" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="E245" s="6">
+        <v>250</v>
+      </c>
+      <c r="F245" s="6">
+        <v>210</v>
+      </c>
+      <c r="G245" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H245" s="11">
+        <v>1.75</v>
+      </c>
+      <c r="I245" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J245" s="11">
+        <f t="shared" si="17"/>
+        <v>-0.5</v>
+      </c>
+      <c r="K245" s="11">
+        <f t="shared" si="14"/>
+        <v>56.350000000000009</v>
+      </c>
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A246" s="8"/>
-      <c r="B246" s="8"/>
-      <c r="C246" s="8"/>
-      <c r="D246" s="8"/>
-      <c r="E246" s="6"/>
-      <c r="F246" s="6"/>
-      <c r="G246" s="11"/>
-      <c r="H246" s="11"/>
-      <c r="I246" s="8"/>
-      <c r="J246" s="11"/>
-      <c r="K246" s="11"/>
+      <c r="A246" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B246" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C246" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D246" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="E246" s="6">
+        <v>120</v>
+      </c>
+      <c r="F246" s="6">
+        <v>115</v>
+      </c>
+      <c r="G246" s="11">
+        <v>2</v>
+      </c>
+      <c r="H246" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I246" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J246" s="11">
+        <f t="shared" si="17"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="K246" s="11">
+        <f t="shared" si="14"/>
+        <v>58.750000000000007</v>
+      </c>
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A247" s="8"/>
-      <c r="B247" s="8"/>
-      <c r="C247" s="8"/>
-      <c r="D247" s="8"/>
-      <c r="E247" s="6"/>
-      <c r="F247" s="6"/>
-      <c r="G247" s="11"/>
-      <c r="H247" s="11"/>
-      <c r="I247" s="8"/>
-      <c r="J247" s="11"/>
-      <c r="K247" s="11"/>
+      <c r="A247" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B247" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C247" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D247" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="E247" s="6">
+        <v>145</v>
+      </c>
+      <c r="F247" s="6">
+        <v>115</v>
+      </c>
+      <c r="G247" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H247" s="11">
+        <v>3.68</v>
+      </c>
+      <c r="I247" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J247" s="11">
+        <f t="shared" si="17"/>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K247" s="11">
+        <f t="shared" si="14"/>
+        <v>60.930000000000007</v>
+      </c>
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A248" s="8"/>
-      <c r="B248" s="8"/>
-      <c r="C248" s="8"/>
-      <c r="D248" s="8"/>
-      <c r="E248" s="6"/>
-      <c r="F248" s="6"/>
-      <c r="G248" s="11"/>
-      <c r="H248" s="11"/>
-      <c r="I248" s="8"/>
-      <c r="J248" s="11"/>
-      <c r="K248" s="11"/>
+      <c r="A248" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B248" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="C248" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D248" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="E248" s="6">
+        <v>125</v>
+      </c>
+      <c r="F248" s="6">
+        <v>125</v>
+      </c>
+      <c r="G248" s="11">
+        <v>1</v>
+      </c>
+      <c r="H248" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="I248" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J248" s="11">
+        <f t="shared" si="17"/>
+        <v>1.25</v>
+      </c>
+      <c r="K248" s="11">
+        <f t="shared" si="14"/>
+        <v>62.180000000000007</v>
+      </c>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A249" s="8"/>
-      <c r="B249" s="8"/>
-      <c r="C249" s="8"/>
-      <c r="D249" s="8"/>
-      <c r="E249" s="6"/>
-      <c r="F249" s="6"/>
-      <c r="G249" s="11"/>
-      <c r="H249" s="11"/>
-      <c r="I249" s="8"/>
-      <c r="J249" s="11"/>
-      <c r="K249" s="11"/>
+      <c r="A249" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B249" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C249" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D249" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="E249" s="6">
+        <v>110</v>
+      </c>
+      <c r="F249" s="6">
+        <v>110</v>
+      </c>
+      <c r="G249" s="11">
+        <v>3</v>
+      </c>
+      <c r="H249" s="11">
+        <v>6.3</v>
+      </c>
+      <c r="I249" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J249" s="11">
+        <f t="shared" si="17"/>
+        <v>3.3</v>
+      </c>
+      <c r="K249" s="11">
+        <f t="shared" si="14"/>
+        <v>65.48</v>
+      </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A250" s="8"/>
-      <c r="B250" s="8"/>
-      <c r="C250" s="8"/>
-      <c r="D250" s="8"/>
-      <c r="E250" s="6"/>
-      <c r="F250" s="6"/>
-      <c r="G250" s="11"/>
-      <c r="H250" s="11"/>
-      <c r="I250" s="8"/>
-      <c r="J250" s="11"/>
-      <c r="K250" s="11"/>
+      <c r="A250" s="7">
+        <v>44937</v>
+      </c>
+      <c r="B250" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C250" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D250" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="E250" s="6">
+        <v>-130</v>
+      </c>
+      <c r="F250" s="6">
+        <v>-130</v>
+      </c>
+      <c r="G250" s="11">
+        <v>2</v>
+      </c>
+      <c r="H250" s="11">
+        <v>3.54</v>
+      </c>
+      <c r="I250" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J250" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K250" s="11">
+        <f t="shared" si="14"/>
+        <v>63.480000000000004</v>
+      </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A251" s="8"/>
-      <c r="B251" s="8"/>
-      <c r="C251" s="8"/>
-      <c r="D251" s="8"/>
-      <c r="E251" s="6"/>
-      <c r="F251" s="6"/>
-      <c r="G251" s="11"/>
-      <c r="H251" s="11"/>
-      <c r="I251" s="8"/>
-      <c r="J251" s="11"/>
-      <c r="K251" s="11"/>
+      <c r="A251" s="7">
+        <v>44938</v>
+      </c>
+      <c r="B251" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="C251" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D251" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E251" s="6">
+        <v>-175</v>
+      </c>
+      <c r="F251" s="6">
+        <v>-210</v>
+      </c>
+      <c r="G251" s="11">
+        <v>3</v>
+      </c>
+      <c r="H251" s="11">
+        <v>4.71</v>
+      </c>
+      <c r="I251" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J251" s="11">
+        <f t="shared" si="17"/>
+        <v>1.71</v>
+      </c>
+      <c r="K251" s="11">
+        <f t="shared" si="14"/>
+        <v>65.19</v>
+      </c>
     </row>
     <row r="252" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A252" s="8"/>
-      <c r="B252" s="8"/>
-      <c r="C252" s="8"/>
-      <c r="D252" s="8"/>
-      <c r="E252" s="6"/>
-      <c r="F252" s="6"/>
-      <c r="G252" s="11"/>
-      <c r="H252" s="11"/>
-      <c r="I252" s="8"/>
-      <c r="J252" s="11"/>
-      <c r="K252" s="11"/>
+      <c r="A252" s="7">
+        <v>44938</v>
+      </c>
+      <c r="B252" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C252" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D252" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="E252" s="6">
+        <v>-145</v>
+      </c>
+      <c r="F252" s="6">
+        <v>-120</v>
+      </c>
+      <c r="G252" s="11">
+        <v>5</v>
+      </c>
+      <c r="H252" s="11">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="I252" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J252" s="11">
+        <f t="shared" si="17"/>
+        <v>-5</v>
+      </c>
+      <c r="K252" s="11">
+        <f t="shared" si="14"/>
+        <v>60.19</v>
+      </c>
     </row>
     <row r="253" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A253" s="8"/>
-      <c r="B253" s="8"/>
-      <c r="C253" s="8"/>
-      <c r="D253" s="8"/>
-      <c r="E253" s="6"/>
-      <c r="F253" s="6"/>
-      <c r="G253" s="11"/>
-      <c r="H253" s="11"/>
-      <c r="I253" s="8"/>
-      <c r="J253" s="11"/>
-      <c r="K253" s="11"/>
+      <c r="A253" s="7">
+        <v>44938</v>
+      </c>
+      <c r="B253" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C253" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D253" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="E253" s="6">
+        <v>140</v>
+      </c>
+      <c r="F253" s="6">
+        <v>115</v>
+      </c>
+      <c r="G253" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H253" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="I253" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J253" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K253" s="11">
+        <f t="shared" si="14"/>
+        <v>58.69</v>
+      </c>
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A254" s="8"/>
-      <c r="B254" s="8"/>
-      <c r="C254" s="8"/>
-      <c r="D254" s="8"/>
-      <c r="E254" s="6"/>
-      <c r="F254" s="6"/>
-      <c r="G254" s="11"/>
-      <c r="H254" s="11"/>
-      <c r="I254" s="8"/>
-      <c r="J254" s="11"/>
-      <c r="K254" s="11"/>
+      <c r="A254" s="7">
+        <v>44939</v>
+      </c>
+      <c r="B254" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="C254" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D254" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="E254" s="6">
+        <v>170</v>
+      </c>
+      <c r="F254" s="6">
+        <v>145</v>
+      </c>
+      <c r="G254" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="H254" s="11">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="I254" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J254" s="11">
+        <f t="shared" si="17"/>
+        <v>5.9499999999999993</v>
+      </c>
+      <c r="K254" s="11">
+        <f t="shared" si="14"/>
+        <v>64.64</v>
+      </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A255" s="8"/>
-      <c r="B255" s="8"/>
-      <c r="C255" s="8"/>
-      <c r="D255" s="8"/>
-      <c r="E255" s="6"/>
-      <c r="F255" s="6"/>
-      <c r="G255" s="11"/>
-      <c r="H255" s="11"/>
-      <c r="I255" s="8"/>
-      <c r="J255" s="11"/>
-      <c r="K255" s="11"/>
+      <c r="A255" s="7">
+        <v>44939</v>
+      </c>
+      <c r="B255" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="C255" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D255" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E255" s="6">
+        <v>135</v>
+      </c>
+      <c r="F255" s="6">
+        <v>135</v>
+      </c>
+      <c r="G255" s="11">
+        <v>3</v>
+      </c>
+      <c r="H255" s="11">
+        <v>7.05</v>
+      </c>
+      <c r="I255" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J255" s="11">
+        <f t="shared" si="17"/>
+        <v>4.05</v>
+      </c>
+      <c r="K255" s="11">
+        <f t="shared" si="14"/>
+        <v>68.69</v>
+      </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A256" s="8"/>
-      <c r="B256" s="8"/>
-      <c r="C256" s="8"/>
-      <c r="D256" s="8"/>
-      <c r="E256" s="6"/>
-      <c r="F256" s="6"/>
-      <c r="G256" s="11"/>
-      <c r="H256" s="11"/>
-      <c r="I256" s="8"/>
-      <c r="J256" s="11"/>
-      <c r="K256" s="11"/>
+      <c r="A256" s="7">
+        <v>44939</v>
+      </c>
+      <c r="B256" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="C256" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D256" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="E256" s="6">
+        <v>650</v>
+      </c>
+      <c r="F256" s="6">
+        <v>725</v>
+      </c>
+      <c r="G256" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H256" s="11">
+        <v>11.25</v>
+      </c>
+      <c r="I256" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J256" s="11">
+        <f t="shared" si="17"/>
+        <v>-1.5</v>
+      </c>
+      <c r="K256" s="11">
+        <f t="shared" si="14"/>
+        <v>67.19</v>
+      </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A257" s="8"/>
-      <c r="B257" s="8"/>
-      <c r="C257" s="8"/>
-      <c r="D257" s="8"/>
-      <c r="E257" s="6"/>
-      <c r="F257" s="6"/>
-      <c r="G257" s="11"/>
-      <c r="H257" s="11"/>
-      <c r="I257" s="8"/>
-      <c r="J257" s="11"/>
-      <c r="K257" s="11"/>
+      <c r="A257" s="7">
+        <v>44940</v>
+      </c>
+      <c r="B257" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="C257" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D257" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="E257" s="6">
+        <v>135</v>
+      </c>
+      <c r="F257" s="6">
+        <v>120</v>
+      </c>
+      <c r="G257" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="H257" s="11">
+        <v>15.29</v>
+      </c>
+      <c r="I257" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J257" s="11">
+        <f t="shared" si="17"/>
+        <v>-6.5</v>
+      </c>
+      <c r="K257" s="11">
+        <f t="shared" si="14"/>
+        <v>60.69</v>
+      </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A258" s="8"/>
-      <c r="B258" s="8"/>
-      <c r="C258" s="8"/>
-      <c r="D258" s="8"/>
-      <c r="E258" s="6"/>
-      <c r="F258" s="6"/>
-      <c r="G258" s="11"/>
-      <c r="H258" s="11"/>
-      <c r="I258" s="8"/>
-      <c r="J258" s="11"/>
-      <c r="K258" s="11"/>
+      <c r="A258" s="7">
+        <v>44940</v>
+      </c>
+      <c r="B258" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C258" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D258" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E258" s="6">
+        <v>205</v>
+      </c>
+      <c r="F258" s="6">
+        <v>205</v>
+      </c>
+      <c r="G258" s="11">
+        <v>2</v>
+      </c>
+      <c r="H258" s="11">
+        <v>6.1</v>
+      </c>
+      <c r="I258" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J258" s="11">
+        <f t="shared" si="17"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K258" s="11">
+        <f t="shared" ref="K258:K268" si="19">K257+J258</f>
+        <v>64.789999999999992</v>
+      </c>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A259" s="8"/>
-      <c r="B259" s="8"/>
-      <c r="C259" s="8"/>
-      <c r="D259" s="8"/>
-      <c r="E259" s="6"/>
-      <c r="F259" s="6"/>
-      <c r="G259" s="11"/>
-      <c r="H259" s="11"/>
-      <c r="I259" s="8"/>
-      <c r="J259" s="11"/>
-      <c r="K259" s="11"/>
+      <c r="A259" s="7">
+        <v>44940</v>
+      </c>
+      <c r="B259" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="C259" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D259" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="E259" s="6">
+        <v>220</v>
+      </c>
+      <c r="F259" s="6">
+        <v>220</v>
+      </c>
+      <c r="G259" s="11">
+        <v>2</v>
+      </c>
+      <c r="H259" s="11">
+        <v>6.4</v>
+      </c>
+      <c r="I259" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J259" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K259" s="11">
+        <f t="shared" si="19"/>
+        <v>62.789999999999992</v>
+      </c>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A260" s="8"/>
-      <c r="B260" s="8"/>
-      <c r="C260" s="8"/>
-      <c r="D260" s="8"/>
-      <c r="E260" s="6"/>
-      <c r="F260" s="6"/>
-      <c r="G260" s="11"/>
-      <c r="H260" s="11"/>
-      <c r="I260" s="8"/>
-      <c r="J260" s="11"/>
-      <c r="K260" s="11"/>
+      <c r="A260" s="7">
+        <v>44940</v>
+      </c>
+      <c r="B260" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="C260" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D260" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="E260" s="6">
+        <v>135</v>
+      </c>
+      <c r="F260" s="6">
+        <v>135</v>
+      </c>
+      <c r="G260" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H260" s="11">
+        <v>3.52</v>
+      </c>
+      <c r="I260" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J260" s="11">
+        <f t="shared" si="17"/>
+        <v>2.02</v>
+      </c>
+      <c r="K260" s="11">
+        <f t="shared" si="19"/>
+        <v>64.809999999999988</v>
+      </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A261" s="8"/>
-      <c r="B261" s="8"/>
-      <c r="C261" s="8"/>
-      <c r="D261" s="8"/>
-      <c r="E261" s="6"/>
-      <c r="F261" s="6"/>
-      <c r="G261" s="11"/>
-      <c r="H261" s="11"/>
-      <c r="I261" s="8"/>
-      <c r="J261" s="11"/>
-      <c r="K261" s="11"/>
+      <c r="A261" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B261" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="C261" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D261" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E261" s="6">
+        <v>360</v>
+      </c>
+      <c r="F261" s="6">
+        <v>350</v>
+      </c>
+      <c r="G261" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="H261" s="11">
+        <v>11.5</v>
+      </c>
+      <c r="I261" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J261" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K261" s="11">
+        <f t="shared" si="19"/>
+        <v>64.809999999999988</v>
+      </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A262" s="8"/>
-      <c r="B262" s="8"/>
-      <c r="C262" s="8"/>
-      <c r="D262" s="8"/>
-      <c r="E262" s="6"/>
-      <c r="F262" s="6"/>
-      <c r="G262" s="11"/>
-      <c r="H262" s="11"/>
-      <c r="I262" s="8"/>
-      <c r="J262" s="11"/>
-      <c r="K262" s="11"/>
+      <c r="A262" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B262" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="C262" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D262" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="E262" s="6">
+        <v>120</v>
+      </c>
+      <c r="F262" s="6">
+        <v>120</v>
+      </c>
+      <c r="G262" s="11">
+        <v>3</v>
+      </c>
+      <c r="H262" s="11">
+        <v>6.6</v>
+      </c>
+      <c r="I262" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J262" s="11">
+        <f t="shared" si="17"/>
+        <v>-3</v>
+      </c>
+      <c r="K262" s="11">
+        <f t="shared" si="19"/>
+        <v>61.809999999999988</v>
+      </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A263" s="8"/>
-      <c r="B263" s="8"/>
-      <c r="C263" s="8"/>
-      <c r="D263" s="8"/>
-      <c r="E263" s="6"/>
-      <c r="F263" s="6"/>
-      <c r="G263" s="11"/>
-      <c r="H263" s="11"/>
-      <c r="I263" s="8"/>
-      <c r="J263" s="11"/>
-      <c r="K263" s="11"/>
+      <c r="A263" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B263" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="C263" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D263" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E263" s="6">
+        <v>325</v>
+      </c>
+      <c r="F263" s="6">
+        <v>280</v>
+      </c>
+      <c r="G263" s="11">
+        <v>2</v>
+      </c>
+      <c r="H263" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="I263" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J263" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K263" s="11">
+        <f t="shared" si="19"/>
+        <v>59.809999999999988</v>
+      </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A264" s="8"/>
-      <c r="B264" s="8"/>
-      <c r="C264" s="8"/>
-      <c r="D264" s="8"/>
-      <c r="E264" s="6"/>
-      <c r="F264" s="6"/>
-      <c r="G264" s="11"/>
-      <c r="H264" s="11"/>
-      <c r="I264" s="8"/>
-      <c r="J264" s="11"/>
-      <c r="K264" s="11"/>
+      <c r="A264" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B264" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="C264" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D264" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="E264" s="6">
+        <v>130</v>
+      </c>
+      <c r="F264" s="6">
+        <v>130</v>
+      </c>
+      <c r="G264" s="11">
+        <v>5</v>
+      </c>
+      <c r="H264" s="11">
+        <v>11.5</v>
+      </c>
+      <c r="I264" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J264" s="11">
+        <f t="shared" si="17"/>
+        <v>6.5</v>
+      </c>
+      <c r="K264" s="11">
+        <f t="shared" si="19"/>
+        <v>66.309999999999988</v>
+      </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A265" s="8"/>
-      <c r="B265" s="8"/>
-      <c r="C265" s="8"/>
-      <c r="D265" s="8"/>
-      <c r="E265" s="6"/>
-      <c r="F265" s="6"/>
-      <c r="G265" s="11"/>
-      <c r="H265" s="11"/>
-      <c r="I265" s="8"/>
-      <c r="J265" s="11"/>
-      <c r="K265" s="11"/>
+      <c r="A265" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B265" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="C265" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="D265" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E265" s="6">
+        <v>-105</v>
+      </c>
+      <c r="F265" s="6">
+        <v>105</v>
+      </c>
+      <c r="G265" s="11">
+        <v>3</v>
+      </c>
+      <c r="H265" s="11">
+        <v>6.15</v>
+      </c>
+      <c r="I265" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J265" s="11">
+        <f t="shared" si="17"/>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="K265" s="11">
+        <f t="shared" si="19"/>
+        <v>69.459999999999994</v>
+      </c>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A266" s="8"/>
-      <c r="B266" s="8"/>
-      <c r="C266" s="8"/>
-      <c r="D266" s="8"/>
-      <c r="E266" s="6"/>
-      <c r="F266" s="6"/>
-      <c r="G266" s="11"/>
-      <c r="H266" s="11"/>
-      <c r="I266" s="8"/>
-      <c r="J266" s="11"/>
-      <c r="K266" s="11"/>
+      <c r="A266" s="7">
+        <v>44942</v>
+      </c>
+      <c r="B266" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="C266" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D266" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E266" s="6">
+        <v>190</v>
+      </c>
+      <c r="F266" s="6">
+        <v>200</v>
+      </c>
+      <c r="G266" s="11">
+        <v>3</v>
+      </c>
+      <c r="H266" s="11">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I266" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J266" s="11">
+        <f t="shared" si="17"/>
+        <v>-3</v>
+      </c>
+      <c r="K266" s="11">
+        <f t="shared" si="19"/>
+        <v>66.459999999999994</v>
+      </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A267" s="8"/>
-      <c r="B267" s="8"/>
-      <c r="C267" s="8"/>
-      <c r="D267" s="8"/>
-      <c r="E267" s="6"/>
-      <c r="F267" s="6"/>
-      <c r="G267" s="11"/>
-      <c r="H267" s="11"/>
-      <c r="I267" s="8"/>
-      <c r="J267" s="11"/>
-      <c r="K267" s="11"/>
+      <c r="A267" s="7">
+        <v>44943</v>
+      </c>
+      <c r="B267" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="C267" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D267" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="E267" s="6">
+        <v>235</v>
+      </c>
+      <c r="F267" s="6">
+        <v>195</v>
+      </c>
+      <c r="G267" s="11">
+        <v>2</v>
+      </c>
+      <c r="H267" s="11">
+        <v>6.7</v>
+      </c>
+      <c r="I267" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J267" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K267" s="11">
+        <f t="shared" si="19"/>
+        <v>64.459999999999994</v>
+      </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A268" s="8"/>
-      <c r="B268" s="8"/>
-      <c r="C268" s="8"/>
-      <c r="D268" s="8"/>
-      <c r="E268" s="6"/>
-      <c r="F268" s="6"/>
-      <c r="G268" s="11"/>
-      <c r="H268" s="11"/>
-      <c r="I268" s="8"/>
-      <c r="J268" s="11"/>
-      <c r="K268" s="11"/>
+      <c r="A268" s="7">
+        <v>44943</v>
+      </c>
+      <c r="B268" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="C268" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D268" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E268" s="6">
+        <v>155</v>
+      </c>
+      <c r="F268" s="6">
+        <v>155</v>
+      </c>
+      <c r="G268" s="11">
+        <v>3</v>
+      </c>
+      <c r="H268" s="11">
+        <v>7.65</v>
+      </c>
+      <c r="I268" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J268" s="11">
+        <f t="shared" si="17"/>
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="K268" s="11">
+        <f t="shared" si="19"/>
+        <v>69.11</v>
+      </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A269" s="8"/>
-      <c r="B269" s="8"/>
-      <c r="C269" s="8"/>
-      <c r="D269" s="8"/>
-      <c r="E269" s="6"/>
-      <c r="F269" s="6"/>
-      <c r="G269" s="11"/>
-      <c r="H269" s="11"/>
-      <c r="I269" s="8"/>
-      <c r="J269" s="11"/>
-      <c r="K269" s="11"/>
+      <c r="A269" s="7">
+        <v>44943</v>
+      </c>
+      <c r="B269" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C269" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D269" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="E269" s="6">
+        <v>110</v>
+      </c>
+      <c r="F269" s="6">
+        <v>-105</v>
+      </c>
+      <c r="G269" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="H269" s="11">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="I269" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J269" s="11">
+        <f t="shared" si="17"/>
+        <v>-4.5</v>
+      </c>
+      <c r="K269" s="11">
+        <f t="shared" ref="K269:K286" si="20">K268+J269</f>
+        <v>64.61</v>
+      </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A270" s="8"/>
-      <c r="B270" s="8"/>
-      <c r="C270" s="8"/>
-      <c r="D270" s="8"/>
-      <c r="E270" s="6"/>
-      <c r="F270" s="6"/>
-      <c r="G270" s="11"/>
-      <c r="H270" s="11"/>
-      <c r="I270" s="8"/>
-      <c r="J270" s="11"/>
-      <c r="K270" s="11"/>
+      <c r="A270" s="7">
+        <v>44943</v>
+      </c>
+      <c r="B270" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="C270" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D270" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="E270" s="6">
+        <v>220</v>
+      </c>
+      <c r="F270" s="6">
+        <v>220</v>
+      </c>
+      <c r="G270" s="11">
+        <v>2</v>
+      </c>
+      <c r="H270" s="11">
+        <v>6.4</v>
+      </c>
+      <c r="I270" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J270" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K270" s="11">
+        <f t="shared" si="20"/>
+        <v>62.61</v>
+      </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A271" s="8"/>
-      <c r="B271" s="8"/>
-      <c r="C271" s="8"/>
-      <c r="D271" s="8"/>
-      <c r="E271" s="6"/>
-      <c r="F271" s="6"/>
-      <c r="G271" s="11"/>
-      <c r="H271" s="11"/>
-      <c r="I271" s="8"/>
-      <c r="J271" s="11"/>
-      <c r="K271" s="11"/>
+      <c r="A271" s="7">
+        <v>44943</v>
+      </c>
+      <c r="B271" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="C271" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D271" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E271" s="6">
+        <v>250</v>
+      </c>
+      <c r="F271" s="6">
+        <v>220</v>
+      </c>
+      <c r="G271" s="11">
+        <v>2</v>
+      </c>
+      <c r="H271" s="11">
+        <v>7</v>
+      </c>
+      <c r="I271" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J271" s="11">
+        <f t="shared" si="17"/>
+        <v>-2</v>
+      </c>
+      <c r="K271" s="11">
+        <f t="shared" si="20"/>
+        <v>60.61</v>
+      </c>
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A272" s="8"/>
-      <c r="B272" s="8"/>
-      <c r="C272" s="8"/>
-      <c r="D272" s="8"/>
-      <c r="E272" s="6"/>
-      <c r="F272" s="6"/>
-      <c r="G272" s="11"/>
-      <c r="H272" s="11"/>
-      <c r="I272" s="8"/>
-      <c r="J272" s="11"/>
-      <c r="K272" s="11"/>
+      <c r="A272" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B272" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="C272" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D272" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="E272" s="6">
+        <v>140</v>
+      </c>
+      <c r="F272" s="6">
+        <v>120</v>
+      </c>
+      <c r="G272" s="11">
+        <v>6</v>
+      </c>
+      <c r="H272" s="11">
+        <v>14.4</v>
+      </c>
+      <c r="I272" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J272" s="11">
+        <f t="shared" si="17"/>
+        <v>8.4</v>
+      </c>
+      <c r="K272" s="11">
+        <f t="shared" si="20"/>
+        <v>69.010000000000005</v>
+      </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A273" s="8"/>
-      <c r="B273" s="8"/>
-      <c r="C273" s="8"/>
-      <c r="D273" s="8"/>
-      <c r="E273" s="6"/>
-      <c r="F273" s="6"/>
-      <c r="G273" s="11"/>
-      <c r="H273" s="11"/>
-      <c r="I273" s="8"/>
-      <c r="J273" s="11"/>
-      <c r="K273" s="11"/>
+      <c r="A273" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B273" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="C273" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D273" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="E273" s="6">
+        <v>-170</v>
+      </c>
+      <c r="F273" s="6">
+        <v>-170</v>
+      </c>
+      <c r="G273" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="H273" s="11">
+        <v>8.74</v>
+      </c>
+      <c r="I273" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J273" s="11">
+        <f t="shared" si="17"/>
+        <v>3.24</v>
+      </c>
+      <c r="K273" s="11">
+        <f t="shared" si="20"/>
+        <v>72.25</v>
+      </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A274" s="8"/>
-      <c r="B274" s="8"/>
-      <c r="C274" s="8"/>
-      <c r="D274" s="8"/>
-      <c r="E274" s="6"/>
-      <c r="F274" s="6"/>
-      <c r="G274" s="11"/>
-      <c r="H274" s="11"/>
-      <c r="I274" s="8"/>
-      <c r="J274" s="11"/>
-      <c r="K274" s="11"/>
+      <c r="A274" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B274" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="C274" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D274" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="E274" s="6">
+        <v>-130</v>
+      </c>
+      <c r="F274" s="6">
+        <v>-125</v>
+      </c>
+      <c r="G274" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="H274" s="11">
+        <v>7.96</v>
+      </c>
+      <c r="I274" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J274" s="11">
+        <f t="shared" si="17"/>
+        <v>3.46</v>
+      </c>
+      <c r="K274" s="11">
+        <f t="shared" si="20"/>
+        <v>75.709999999999994</v>
+      </c>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A275" s="8"/>
-      <c r="B275" s="8"/>
-      <c r="C275" s="8"/>
-      <c r="D275" s="8"/>
-      <c r="E275" s="6"/>
-      <c r="F275" s="6"/>
-      <c r="G275" s="11"/>
-      <c r="H275" s="11"/>
-      <c r="I275" s="8"/>
-      <c r="J275" s="11"/>
-      <c r="K275" s="11"/>
+      <c r="A275" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B275" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="C275" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D275" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="E275" s="6">
+        <v>130</v>
+      </c>
+      <c r="F275" s="6">
+        <v>130</v>
+      </c>
+      <c r="G275" s="11">
+        <v>3</v>
+      </c>
+      <c r="H275" s="11">
+        <v>6.9</v>
+      </c>
+      <c r="I275" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J275" s="11">
+        <f t="shared" si="17"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="K275" s="11">
+        <f t="shared" si="20"/>
+        <v>79.61</v>
+      </c>
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A276" s="8"/>
-      <c r="B276" s="8"/>
-      <c r="C276" s="8"/>
-      <c r="D276" s="8"/>
-      <c r="E276" s="6"/>
-      <c r="F276" s="6"/>
-      <c r="G276" s="11"/>
-      <c r="H276" s="11"/>
-      <c r="I276" s="8"/>
-      <c r="J276" s="11"/>
-      <c r="K276" s="11"/>
+      <c r="A276" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B276" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="C276" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D276" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E276" s="6">
+        <v>350</v>
+      </c>
+      <c r="F276" s="6">
+        <v>350</v>
+      </c>
+      <c r="G276" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="H276" s="11">
+        <v>15.75</v>
+      </c>
+      <c r="I276" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J276" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K276" s="11">
+        <f t="shared" si="20"/>
+        <v>79.61</v>
+      </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A277" s="8"/>
-      <c r="B277" s="8"/>
-      <c r="C277" s="8"/>
-      <c r="D277" s="8"/>
-      <c r="E277" s="6"/>
-      <c r="F277" s="6"/>
-      <c r="G277" s="11"/>
-      <c r="H277" s="11"/>
-      <c r="I277" s="8"/>
-      <c r="J277" s="11"/>
-      <c r="K277" s="11"/>
+      <c r="A277" s="7">
+        <v>44944</v>
+      </c>
+      <c r="B277" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="C277" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D277" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E277" s="6">
+        <v>-150</v>
+      </c>
+      <c r="F277" s="6">
+        <v>-150</v>
+      </c>
+      <c r="G277" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="H277" s="11">
+        <v>5.88</v>
+      </c>
+      <c r="I277" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J277" s="11">
+        <f t="shared" si="17"/>
+        <v>2.38</v>
+      </c>
+      <c r="K277" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A278" s="8"/>
-      <c r="B278" s="8"/>
-      <c r="C278" s="8"/>
-      <c r="D278" s="8"/>
-      <c r="E278" s="6"/>
-      <c r="F278" s="6"/>
-      <c r="G278" s="11"/>
-      <c r="H278" s="11"/>
-      <c r="I278" s="8"/>
-      <c r="J278" s="11"/>
-      <c r="K278" s="11"/>
+      <c r="A278" s="7">
+        <v>44945</v>
+      </c>
+      <c r="B278" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="C278" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D278" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="E278" s="6">
+        <v>275</v>
+      </c>
+      <c r="F278" s="6">
+        <v>275</v>
+      </c>
+      <c r="G278" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="H278" s="11">
+        <v>20.62</v>
+      </c>
+      <c r="I278" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J278" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K278" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A279" s="8"/>
-      <c r="B279" s="8"/>
-      <c r="C279" s="8"/>
-      <c r="D279" s="8"/>
-      <c r="E279" s="6"/>
-      <c r="F279" s="6"/>
-      <c r="G279" s="11"/>
-      <c r="H279" s="11"/>
-      <c r="I279" s="8"/>
-      <c r="J279" s="11"/>
-      <c r="K279" s="11"/>
+      <c r="A279" s="7">
+        <v>44945</v>
+      </c>
+      <c r="B279" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="C279" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D279" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="E279" s="6">
+        <v>210</v>
+      </c>
+      <c r="F279" s="6">
+        <v>220</v>
+      </c>
+      <c r="G279" s="11">
+        <v>2</v>
+      </c>
+      <c r="H279" s="11">
+        <v>6.2</v>
+      </c>
+      <c r="I279" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J279" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K279" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A280" s="8"/>
-      <c r="B280" s="8"/>
-      <c r="C280" s="8"/>
-      <c r="D280" s="8"/>
-      <c r="E280" s="6"/>
-      <c r="F280" s="6"/>
-      <c r="G280" s="11"/>
-      <c r="H280" s="11"/>
-      <c r="I280" s="8"/>
-      <c r="J280" s="11"/>
-      <c r="K280" s="11"/>
+      <c r="A280" s="7">
+        <v>44945</v>
+      </c>
+      <c r="B280" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="C280" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D280" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E280" s="6">
+        <v>140</v>
+      </c>
+      <c r="F280" s="6">
+        <v>140</v>
+      </c>
+      <c r="G280" s="11">
+        <v>7</v>
+      </c>
+      <c r="H280" s="11">
+        <v>16.8</v>
+      </c>
+      <c r="I280" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J280" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="K280" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A281" s="8"/>
-      <c r="B281" s="8"/>
-      <c r="C281" s="8"/>
-      <c r="D281" s="8"/>
-      <c r="E281" s="6"/>
-      <c r="F281" s="6"/>
-      <c r="G281" s="11"/>
-      <c r="H281" s="11"/>
-      <c r="I281" s="8"/>
-      <c r="J281" s="11"/>
-      <c r="K281" s="11"/>
+      <c r="A281" s="7">
+        <v>44945</v>
+      </c>
+      <c r="B281" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="C281" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D281" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E281" s="6">
+        <v>135</v>
+      </c>
+      <c r="F281" s="6">
+        <v>135</v>
+      </c>
+      <c r="G281" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="H281" s="11">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="I281" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J281" s="11">
+        <f t="shared" ref="J281" si="21">IF(I281="Pending", 0,IF(I281="Win",H281-G281,-1*G281))</f>
+        <v>0</v>
+      </c>
+      <c r="K281" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="8"/>
@@ -13155,7 +14976,10 @@
       <c r="H282" s="11"/>
       <c r="I282" s="8"/>
       <c r="J282" s="11"/>
-      <c r="K282" s="11"/>
+      <c r="K282" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="8"/>
@@ -13168,7 +14992,10 @@
       <c r="H283" s="11"/>
       <c r="I283" s="8"/>
       <c r="J283" s="11"/>
-      <c r="K283" s="11"/>
+      <c r="K283" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="8"/>
@@ -13181,7 +15008,10 @@
       <c r="H284" s="11"/>
       <c r="I284" s="8"/>
       <c r="J284" s="11"/>
-      <c r="K284" s="11"/>
+      <c r="K284" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="8"/>
@@ -13194,7 +15024,10 @@
       <c r="H285" s="11"/>
       <c r="I285" s="8"/>
       <c r="J285" s="11"/>
-      <c r="K285" s="11"/>
+      <c r="K285" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="8"/>
@@ -13207,7 +15040,10 @@
       <c r="H286" s="11"/>
       <c r="I286" s="8"/>
       <c r="J286" s="11"/>
-      <c r="K286" s="11"/>
+      <c r="K286" s="11">
+        <f t="shared" si="20"/>
+        <v>81.99</v>
+      </c>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="8"/>
@@ -14742,110 +16578,6 @@
       <c r="I404" s="8"/>
       <c r="J404" s="11"/>
       <c r="K404" s="11"/>
-    </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A405" s="8"/>
-      <c r="B405" s="8"/>
-      <c r="C405" s="8"/>
-      <c r="D405" s="8"/>
-      <c r="E405" s="6"/>
-      <c r="F405" s="6"/>
-      <c r="G405" s="11"/>
-      <c r="H405" s="11"/>
-      <c r="I405" s="8"/>
-      <c r="J405" s="11"/>
-      <c r="K405" s="11"/>
-    </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A406" s="8"/>
-      <c r="B406" s="8"/>
-      <c r="C406" s="8"/>
-      <c r="D406" s="8"/>
-      <c r="E406" s="6"/>
-      <c r="F406" s="6"/>
-      <c r="G406" s="11"/>
-      <c r="H406" s="11"/>
-      <c r="I406" s="8"/>
-      <c r="J406" s="11"/>
-      <c r="K406" s="11"/>
-    </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A407" s="8"/>
-      <c r="B407" s="8"/>
-      <c r="C407" s="8"/>
-      <c r="D407" s="8"/>
-      <c r="E407" s="6"/>
-      <c r="F407" s="6"/>
-      <c r="G407" s="11"/>
-      <c r="H407" s="11"/>
-      <c r="I407" s="8"/>
-      <c r="J407" s="11"/>
-      <c r="K407" s="11"/>
-    </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A408" s="8"/>
-      <c r="B408" s="8"/>
-      <c r="C408" s="8"/>
-      <c r="D408" s="8"/>
-      <c r="E408" s="6"/>
-      <c r="F408" s="6"/>
-      <c r="G408" s="11"/>
-      <c r="H408" s="11"/>
-      <c r="I408" s="8"/>
-      <c r="J408" s="11"/>
-      <c r="K408" s="11"/>
-    </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A409" s="8"/>
-      <c r="B409" s="8"/>
-      <c r="C409" s="8"/>
-      <c r="D409" s="8"/>
-      <c r="E409" s="6"/>
-      <c r="F409" s="6"/>
-      <c r="G409" s="11"/>
-      <c r="H409" s="11"/>
-      <c r="I409" s="8"/>
-      <c r="J409" s="11"/>
-      <c r="K409" s="11"/>
-    </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A410" s="8"/>
-      <c r="B410" s="8"/>
-      <c r="C410" s="8"/>
-      <c r="D410" s="8"/>
-      <c r="E410" s="6"/>
-      <c r="F410" s="6"/>
-      <c r="G410" s="11"/>
-      <c r="H410" s="11"/>
-      <c r="I410" s="8"/>
-      <c r="J410" s="11"/>
-      <c r="K410" s="11"/>
-    </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A411" s="8"/>
-      <c r="B411" s="8"/>
-      <c r="C411" s="8"/>
-      <c r="D411" s="8"/>
-      <c r="E411" s="6"/>
-      <c r="F411" s="6"/>
-      <c r="G411" s="11"/>
-      <c r="H411" s="11"/>
-      <c r="I411" s="8"/>
-      <c r="J411" s="11"/>
-      <c r="K411" s="11"/>
-    </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A412" s="8"/>
-      <c r="B412" s="8"/>
-      <c r="C412" s="8"/>
-      <c r="D412" s="8"/>
-      <c r="E412" s="6"/>
-      <c r="F412" s="6"/>
-      <c r="G412" s="11"/>
-      <c r="H412" s="11"/>
-      <c r="I412" s="8"/>
-      <c r="J412" s="11"/>
-      <c r="K412" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>